<commit_message>
Generate Report for Handback
</commit_message>
<xml_diff>
--- a/ol-handback/OpenLocalizationOrg/core-docs/master/localization-status.xlsx
+++ b/ol-handback/OpenLocalizationOrg/core-docs/master/localization-status.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="565">
   <si>
     <t>File Name</t>
   </si>
@@ -45,7 +45,7 @@
     <t/>
   </si>
   <si>
-    <t>Ready for handoff</t>
+    <t>Handed back: in sync with en-US</t>
   </si>
   <si>
     <t>2016-08-09 01:36:38</t>
@@ -1032,625 +1032,628 @@
     <t>ISSUE_TEMPLATE.077785ab14de46dc6954b7391cc1c58a4474b00a.zh-cn.xlf</t>
   </si>
   <si>
+    <t>2016-08-09 01:53:06</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>PULL_REQUEST_TEMPLATE.8a821da07bda465c58da2993c9218ce5b6db0f19.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>index.016e936c0a212c565bbe5d954bc1404211d04e59.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>apidoc</t>
+  </si>
+  <si>
+    <t>Microsoft.CSharp.RuntimeBinder.Binder.overwrite.5e9175ea4f9d65f5b54ec91db662901d9ef470f7.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\about</t>
+  </si>
+  <si>
+    <t>index.64c99b0d73312cb06eb68b34f3a937345fb389cb.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>products.ebdb86234bc94877f6161f2a1a795c27bd341f8c.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core</t>
+  </si>
+  <si>
+    <t>app-types.0987f6c1d2b5234f56598b7a3697680f81a70fef.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\deploying</t>
+  </si>
+  <si>
+    <t>creating-nuget-packages.c475fc5750d46475259536fb5517ba3038e56d3b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.67220a95f2cab22dfe4dd5dc24845270f94ccf92.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>reducing-dependencies.71640f63ca24d0088f5f9191f05950b16b59c636.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>getting-started.367dc2930aef7c77a5a117c7bc3b6ecc0f43b683.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.e290000c29850e3aea16828e0cef48f5e6ff9019.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\media\packages</t>
+  </si>
+  <si>
+    <t>56bd387874a315cb6da9a292adfb81d95a6bb76e.png</t>
+  </si>
+  <si>
+    <t>True(Dependency)</t>
+  </si>
+  <si>
+    <t>migrating-from-dnx.24d16746eac67884186db7c106ff543d42acccbf.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>packages.c78b9979b9c0b8b243fe2617dc387910a923c545.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\porting</t>
+  </si>
+  <si>
+    <t>index.f7621ba81749b6d65c0e169c188d7df7411e4481.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>libraries.3132f48c3a1585e48f7b575dee2897aa14ab74ba.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\porting\media\project-structure</t>
+  </si>
+  <si>
+    <t>b8076d6effa23eac989ed463b108ab609d72ee81.png</t>
+  </si>
+  <si>
+    <t>53c2807b4930672a4dca14af87586093931c40a7.png</t>
+  </si>
+  <si>
+    <t>e8df3c3cca65bf169a014f30b97869a420065f61.png</t>
+  </si>
+  <si>
+    <t>9e5b560d111542f9e61b18cfd9143d0adb9325e5.png</t>
+  </si>
+  <si>
+    <t>project-structure.0e627b906b2a5022d4e625806ceb3172f393040f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>third-party-deps.18ddccf56c882bc7efa2138e10972ab6228ccca8.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>rid-catalog.dbc1e8e6dfdab6be7c33b1586c1d7bc02125dcb9.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>sdk.9c3255d4577e69d6aee70730290944dc9d2da45d.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\testing</t>
+  </si>
+  <si>
+    <t>index.874b2218474cbbb7738dd697aef54bd275718c7c.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>unit-testing-with-dotnet-test.ac456b50cdaf9eaf743ffc66cb459ad9ec585b4b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\tools</t>
+  </si>
+  <si>
+    <t>dotnet-build.49fca737e1e9cf15e960c32f3dee6836c99b8799.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-install-script.6e82ea7bd7b9b2ea1a835cf96850b7989f7c8b2e.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-new.1c4e72c8a865272c8db60fcd510833b3cc8c3f2b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-pack.e5a20bb4d381ee05ca6581a01e060b08c6a91585.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-publish.fb8bc7a4fcfdbfa813a4cb6f6c5fc58b0192cf0f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-restore.0c97b14cf1c3a5b0dcfa5635a6283cdf555c65c5.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-run.8b62f2b7a8242b4d661b42e711a1fe139f09a3c5.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet-test.6f5b0518d5e55e059424b5a3544f93a6d2f900ea.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>dotnet.9b94b9183f41bc72bf2612cb95e9088edd32db8c.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>extensibility.a6b11625791e2c09d915852be474526dc9487104.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>global-json.bcf96f7f0bed50cf3a64cde9a9077d38563d8cfa.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.69eda7c852108c787b6219d9b8523599a75f6f4f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\tools\media\test-protocol</t>
+  </si>
+  <si>
+    <t>ef6d86dc7da862a2a61112c666acbd4fa48b22c8.png</t>
+  </si>
+  <si>
+    <t>63bf500252fc112edf2e2bf9293b7fdcf08cc834.png</t>
+  </si>
+  <si>
+    <t>project-json.bb712b7268803d4ec572b6dda9a808d28af173a9.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>telemetry.1c2d2f66e2f7ddb65a3162d84b46390eaf6c700e.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>test-protocol.a59cc173f516589fa2bcb6d209f8d7e699990a82.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>using-ci-with-cli.aeb9bf03ecb439e411bf19a7b3b234950e477308.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\tutorials</t>
+  </si>
+  <si>
+    <t>aspnet-core.0ce12fb95da3389d420f8d760beddf56ba76296f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.71dad99a3d8a9a5457c33f8b214681ce0bb0e302.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>libraries.9cfbfeb7612cd8533c4ca1fee0c3e06739154905.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>managing-package-dependency-versions.106313d312f08157767943a637cbc902d4a5d092.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\tutorials\media\target-dotnetcore-with-msbuild</t>
+  </si>
+  <si>
+    <t>d990a7f1678d37de1e1278e6c7cbe72f68399ad9.png</t>
+  </si>
+  <si>
+    <t>ff917d73261fd1657b3952873f3911c8ec9927f4.png</t>
+  </si>
+  <si>
+    <t>docs\core\tutorials\media\using-on-macos</t>
+  </si>
+  <si>
+    <t>80b1c027b9056ff4cdefb6c8730dbea2c5234404.png</t>
+  </si>
+  <si>
+    <t>target-dotnetcore-with-msbuild.89a13906467e804ceb90862ef0993a92e3f97334.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>using-on-macos.3d5cac8bdb9c8dbdda504aa6310f220a1ec07af3.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>using-on-windows.6f63d31d24f569b9ee467193932149ce1f2af726.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>using-with-xplat-cli.734363a82b722d7bc2ca1e083484465a54399ccf.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\core\versions</t>
+  </si>
+  <si>
+    <t>index.b30cf6bccbcaf31708d07e58451f5973b2020242.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>windows-prerequisites.8a7e42c4e05f933f36694fb44fe90ca4e73ec886.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\csharp</t>
+  </si>
+  <si>
+    <t>async.fb7e6562a96b068ce8f188a9a01a1a350b3786e2.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>csharp-6.f054f259d03c8f6ad7cfe33e83ae0905073abc73.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegate-class.04469eb80d6e6aac34f65fea453287188e1b66cd.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegates-events.13b9ae431dc65e962472a9f089cbc607444a0d11.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegates-overview.1032836974f9b23c8a790845708e68c7ac0dc8e3.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegates-patterns.b1cf7308c00cf85b704eceac928d65c7e05cb22b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegates-strongly-typed.49efe714f5cb0e4603fd3cf597d1b9072ef24ecf.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>distinguish-delegates-events.0b74be0746b04d724995663f41511b53c1d4f320.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>event-pattern.69c0983c2624f8e9ec96cde0ac1b457a7d345431.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>events-overview.6895286198c338fe5f27989a87bcbb3e51a642d7.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-classes.84f9c682074e9ad5b3718dd6c9133967b83fe7e2.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-building.4b597d1002b4396ecb33f06f4038cc77361ad2af.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-execution.a8b98bacf0a0bfe629117ad7acd6c10f2905b543.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-explained.062cd4b7229730802fad95bbc61398787daac4c4.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-interpreting.1327c85cae58c3091fe9fc6a1b10715a689ed97e.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-summary.201ee5f6028d637ae1aa2b18e61d2521c52a79f8.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees-translating.94b9bd5a171e1ce9852d2721f9e655d5394de549.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>expression-trees.b39d60187c732853fe485b97eac41692c8dd260c.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>implicitly-typed-lambda-expressions.60e7a9f683139131180bf8e2ae766488526091ca.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>indexers.6ee3f5f37dda8e514c40a01ebdc41e254b42f481.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>iterators.0df40ea5c68ac8561e5021c811e46e560573717c.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>modern-events.02c7181f2ca23448d3e8c68b8581108a34db8312.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>properties.51df8ec1803c024078778aa18555ebc8d5ee81d2.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\csharp\tutorials</t>
+  </si>
+  <si>
+    <t>console-teleprompter.12301eb0699d2d4b5fe67e8251d79b24baedc9ee.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>console-webapiclient.df7cf3ea50355e6f454d41cbd18e38d4003428bd.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.e6f14bd15d9ba180b914a2e448fc867ab3f8c918.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>microservices.429b8aaae4aa1be23a47ef5e3fdae81a433f6e6d.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>working-with-linq.3aaea936956981bacf801f58a14b527f4ae692b6.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\fsharp</t>
+  </si>
+  <si>
+    <t>async.67a4c4cbce5eb33ce073e5fc5a9df5d06342e23b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>getting-started-netcore.ad81c83417296a1870ef09d6e056dc6d453f52b2.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.b0ceeb7aea312772827f7087f8a937edf1e7ed4d.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\images</t>
+  </si>
+  <si>
+    <t>6ee6a35fa247dfe951f4df97818784b30600d543.png</t>
+  </si>
+  <si>
+    <t>docs\samples-and-tutorials</t>
+  </si>
+  <si>
+    <t>index.51c60a85ef778f387438df303e6ad9d2aa9ed3f3.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\standard</t>
+  </si>
+  <si>
+    <t>assembly-format.28db1c2eee4969148649923b2c83a0f9d8295d92.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>async-in-depth.16b4c489db1495cae0a0120c706ec82c79fdaad1.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>async.3c115f3a785660b634cfc3d7818885703e4965aa.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>class-libraries.7dadda8f3a69f2786b36b28fcabb59abbadd8677.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>clr.c6c600ab4fa351d3f792801bca39ed7a8c4d4965.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\standard\collections</t>
+  </si>
+  <si>
+    <t>commonly-used-collection-types.87b05596cbab370816c5e11832c8858aeaa2d9a1.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>comparisons-and-sorts-within-collections.a4814f345079fb61609f208213259d69dfd1affa.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>hashtable-and-dictionary-collection-types.726afc14b9c905ce623486d27942e828bf06348b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.3fe222dc280f54f96b43e0bc742c88c1b6de084a.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>selecting-a-collection-class.aa3adb37e1172576b891f4988de595d66a5011ba.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>sorted-collection-types.ae3aa45904d5407b15dfeb115fbc50a6f2dbaff5.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\standard\collections\threadsafe</t>
+  </si>
+  <si>
+    <t>blockingcollection-overview.47db7fe6b6dc98be9e5d8da6f1869eaa57afe519.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-add-and-remove-items.c77fbc4e7bd3b40ee1e7a82d6c35f6975e1ad92f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-add-and-take-items.74998e2a4567c4ce2e7e8cf4dd3bee2d71a5a9c8.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-add-bounding-and-blocking.d7e8e969f87f13bc8c0b4cb3105c65e5c49d1ed7.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-create-an-object-pool.67d4860ff587e91b4b30745bef2e52949e0b0972.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-use-arrays-of-blockingcollections.d399298da2f3e4c3dbeb438b63d75649f72fdc70.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>how-to-use-foreach-to-remove.5d91710e1ca1f740190d9df9b36fdcb019240590.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.71734fc8bf1ab51eccc74dd34d9e83715727c57b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>when-to-use-a-thread-safe-collection.c906ee56b8927c6037ad35092e542858518686e6.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>when-to-use-generic-collections.ec8a7ec4f16e4f7bd1072115323826242604a56b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>common-type-system.12e59626ca0328f39e75154d0bc212bcbae5a464.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>delegates-lambdas.71df54ba57d186484393e6e83b7a0dca5d9c3a97.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>exceptions.2c65f693d1e10768877aac0dd5db5448f6de5b33.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>framework-libraries.a910059a62e8080f3edc3e6a3141c5392e5f4840.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>frameworks.97b37c9150bfb4e97277c084ce00cbcace849bf8.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>gc-overview.09d3f3c36e4fb85bf89b55884bc8f58e8a4d5080.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>generics.1f8f95282e2b84cdfaeef3636a5944d55a152857.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.8bc2dd87c1d2edcd81672b92705979b37e524590.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>library.387c1e6b222531c2cedef18135a5fa775d5f0452.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>managed-code.c074f35f86522ea606301f15657bc0ee24da87df.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs\standard\media\assembly-format</t>
+  </si>
+  <si>
+    <t>938b47878d90fc32819bbfbae2b5737eab1bf677.png</t>
+  </si>
+  <si>
+    <t>docs\standard\media\portability-analyzer</t>
+  </si>
+  <si>
+    <t>878751ec4663e23a4ea7b70da29e750e222e19fa.png</t>
+  </si>
+  <si>
+    <t>f8208a75ae262d5130b5031bc8562d5b396442ef.png</t>
+  </si>
+  <si>
+    <t>31af85325450edc2abc7ba8dadf618272e81efc4.png</t>
+  </si>
+  <si>
+    <t>docs\standard\media\using-linq</t>
+  </si>
+  <si>
+    <t>e6b57c6b636d3d2d42299083d2b12eb049288e27.png</t>
+  </si>
+  <si>
+    <t>native-interop.8f6566123608155a52a2ab93eca340fe3087fb34.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>numerics.3cae565a7bf0ad930aed72b463f8dc1f484efead.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>portability-analyzer.e8a40fb40eb97b83690447183edbd03a56509a87.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>using-linq.9202ee2cc6a78e5d44a90dd7b156929a14f8fd86.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>docs</t>
+  </si>
+  <si>
+    <t>welcome.cf84032b4d2e283cbf5c69d78077d1efb10a3c58.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>index.b8d322cca13b7303167b216a3efe71db4e1687a1.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>README.8ec9a00bfd09b3190ac6b22251dbb1aa95a0579d.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\console-apps\Fibonacci</t>
+  </si>
+  <si>
+    <t>README.833d3889a48c2604c718bd6cb2dd4b40fb611c09.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\console-apps\FibonacciBetter</t>
+  </si>
+  <si>
+    <t>README.aaf05806fc8bf002d3b366347ba2bd058b82f9b4.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\console-apps\Hello</t>
+  </si>
+  <si>
+    <t>README.2e42c2d62eea4c136751e34541c15ccf9f5a1c2a.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\console-apps\HelloNative</t>
+  </si>
+  <si>
+    <t>README.90878ce4606d18256fdb51ddec9bf70aacfd2fa0.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\console-apps\NewTypes</t>
+  </si>
+  <si>
+    <t>README.a258da1a8e58fc590c32169dad125de335dae304.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\core-projects\libraries</t>
+  </si>
+  <si>
+    <t>README.6deb49b78f2b185dfd36ec0d5e01934d48f66291.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\console-linq</t>
+  </si>
+  <si>
+    <t>README.c1fd3bff6fb8364413ed8f7d51aa552039a25f54.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\console-teleprompter</t>
+  </si>
+  <si>
+    <t>README.b0addf503313b1a99b89254739f8e53852a496e7.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\console-webapiclient</t>
+  </si>
+  <si>
+    <t>README.f3964029da15b075c1a5d79797051a6a2449182d.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\delegates-and-events</t>
+  </si>
+  <si>
+    <t>README.ce0f559e48855520c3e9f6e7f72367231da58b98.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\events</t>
+  </si>
+  <si>
+    <t>README.6efcda3e0b4b04ebc8e2ba8994a543ed0de3356b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\expression-trees</t>
+  </si>
+  <si>
+    <t>README.065c32729da82224a977901d6700fd9f24c159e5.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\indexers</t>
+  </si>
+  <si>
+    <t>README.7ed44e9c8a8d9ca22334b381fd1c40c0880c277b.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\iterators</t>
+  </si>
+  <si>
+    <t>README.5d6c14b3c88e47cf1a390ba2348181637977f186.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\WeatherMicroservice</t>
+  </si>
+  <si>
+    <t>README.6bb043903290a12848181c19f62ec3d21c50140f.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\csharp-language\WeatherMicroservice\wwwroot</t>
+  </si>
+  <si>
+    <t>README.bf3e5645731a4878d9c02fdb008220f45c975f97.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\getting-started\golden</t>
+  </si>
+  <si>
+    <t>README.2cf499dfab094d02d0501c30d2e74e7d1bd21d8a.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\linq\csharp</t>
+  </si>
+  <si>
+    <t>README.67e561b1f112389541ad29652f348dc14d2e4ecc.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>README.ed595a0cdde816cbf12782578f6938544d11577a.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>samples\unit-testing\using-dotnet-test</t>
+  </si>
+  <si>
+    <t>README.c70fdc64850f508e9bf8e2cfd52489f8becd9845.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>styleguide</t>
+  </si>
+  <si>
+    <t>template.f8ef37f92e542c373ce9d5385182d53bb1ce5a60.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>voice-tone.1d6a374e632fbd93441b10f49206a284752ca333.zh-cn.xlf</t>
+  </si>
+  <si>
+    <t>TOC.c5e56b4d05e38e466c0192461b6c26065f810c46.zh-cn.xlf</t>
+  </si>
+  <si>
     <t>0001-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>PULL_REQUEST_TEMPLATE.8a821da07bda465c58da2993c9218ce5b6db0f19.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>api</t>
-  </si>
-  <si>
-    <t>index.016e936c0a212c565bbe5d954bc1404211d04e59.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>apidoc</t>
-  </si>
-  <si>
-    <t>Microsoft.CSharp.RuntimeBinder.Binder.overwrite.5e9175ea4f9d65f5b54ec91db662901d9ef470f7.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\about</t>
-  </si>
-  <si>
-    <t>index.64c99b0d73312cb06eb68b34f3a937345fb389cb.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>products.ebdb86234bc94877f6161f2a1a795c27bd341f8c.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core</t>
-  </si>
-  <si>
-    <t>app-types.0987f6c1d2b5234f56598b7a3697680f81a70fef.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\deploying</t>
-  </si>
-  <si>
-    <t>creating-nuget-packages.c475fc5750d46475259536fb5517ba3038e56d3b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.67220a95f2cab22dfe4dd5dc24845270f94ccf92.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>reducing-dependencies.71640f63ca24d0088f5f9191f05950b16b59c636.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>getting-started.367dc2930aef7c77a5a117c7bc3b6ecc0f43b683.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.e290000c29850e3aea16828e0cef48f5e6ff9019.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\media\packages</t>
-  </si>
-  <si>
-    <t>56bd387874a315cb6da9a292adfb81d95a6bb76e.png</t>
-  </si>
-  <si>
-    <t>True(Dependency)</t>
-  </si>
-  <si>
-    <t>migrating-from-dnx.24d16746eac67884186db7c106ff543d42acccbf.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>packages.c78b9979b9c0b8b243fe2617dc387910a923c545.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\porting</t>
-  </si>
-  <si>
-    <t>index.f7621ba81749b6d65c0e169c188d7df7411e4481.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>libraries.3132f48c3a1585e48f7b575dee2897aa14ab74ba.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\porting\media\project-structure</t>
-  </si>
-  <si>
-    <t>b8076d6effa23eac989ed463b108ab609d72ee81.png</t>
-  </si>
-  <si>
-    <t>53c2807b4930672a4dca14af87586093931c40a7.png</t>
-  </si>
-  <si>
-    <t>e8df3c3cca65bf169a014f30b97869a420065f61.png</t>
-  </si>
-  <si>
-    <t>9e5b560d111542f9e61b18cfd9143d0adb9325e5.png</t>
-  </si>
-  <si>
-    <t>project-structure.0e627b906b2a5022d4e625806ceb3172f393040f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>third-party-deps.18ddccf56c882bc7efa2138e10972ab6228ccca8.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>rid-catalog.dbc1e8e6dfdab6be7c33b1586c1d7bc02125dcb9.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>sdk.9c3255d4577e69d6aee70730290944dc9d2da45d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\testing</t>
-  </si>
-  <si>
-    <t>index.874b2218474cbbb7738dd697aef54bd275718c7c.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>unit-testing-with-dotnet-test.ac456b50cdaf9eaf743ffc66cb459ad9ec585b4b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\tools</t>
-  </si>
-  <si>
-    <t>dotnet-build.49fca737e1e9cf15e960c32f3dee6836c99b8799.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-install-script.6e82ea7bd7b9b2ea1a835cf96850b7989f7c8b2e.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-new.1c4e72c8a865272c8db60fcd510833b3cc8c3f2b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-pack.e5a20bb4d381ee05ca6581a01e060b08c6a91585.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-publish.fb8bc7a4fcfdbfa813a4cb6f6c5fc58b0192cf0f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-restore.0c97b14cf1c3a5b0dcfa5635a6283cdf555c65c5.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-run.8b62f2b7a8242b4d661b42e711a1fe139f09a3c5.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet-test.6f5b0518d5e55e059424b5a3544f93a6d2f900ea.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>dotnet.9b94b9183f41bc72bf2612cb95e9088edd32db8c.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>extensibility.a6b11625791e2c09d915852be474526dc9487104.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>global-json.bcf96f7f0bed50cf3a64cde9a9077d38563d8cfa.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.69eda7c852108c787b6219d9b8523599a75f6f4f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\tools\media\test-protocol</t>
-  </si>
-  <si>
-    <t>ef6d86dc7da862a2a61112c666acbd4fa48b22c8.png</t>
-  </si>
-  <si>
-    <t>63bf500252fc112edf2e2bf9293b7fdcf08cc834.png</t>
-  </si>
-  <si>
-    <t>project-json.bb712b7268803d4ec572b6dda9a808d28af173a9.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>telemetry.1c2d2f66e2f7ddb65a3162d84b46390eaf6c700e.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>test-protocol.a59cc173f516589fa2bcb6d209f8d7e699990a82.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>using-ci-with-cli.aeb9bf03ecb439e411bf19a7b3b234950e477308.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\tutorials</t>
-  </si>
-  <si>
-    <t>aspnet-core.0ce12fb95da3389d420f8d760beddf56ba76296f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.71dad99a3d8a9a5457c33f8b214681ce0bb0e302.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>libraries.9cfbfeb7612cd8533c4ca1fee0c3e06739154905.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>managing-package-dependency-versions.106313d312f08157767943a637cbc902d4a5d092.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\tutorials\media\target-dotnetcore-with-msbuild</t>
-  </si>
-  <si>
-    <t>d990a7f1678d37de1e1278e6c7cbe72f68399ad9.png</t>
-  </si>
-  <si>
-    <t>ff917d73261fd1657b3952873f3911c8ec9927f4.png</t>
-  </si>
-  <si>
-    <t>docs\core\tutorials\media\using-on-macos</t>
-  </si>
-  <si>
-    <t>80b1c027b9056ff4cdefb6c8730dbea2c5234404.png</t>
-  </si>
-  <si>
-    <t>target-dotnetcore-with-msbuild.89a13906467e804ceb90862ef0993a92e3f97334.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>using-on-macos.3d5cac8bdb9c8dbdda504aa6310f220a1ec07af3.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>using-on-windows.6f63d31d24f569b9ee467193932149ce1f2af726.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>using-with-xplat-cli.734363a82b722d7bc2ca1e083484465a54399ccf.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\core\versions</t>
-  </si>
-  <si>
-    <t>index.b30cf6bccbcaf31708d07e58451f5973b2020242.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>windows-prerequisites.8a7e42c4e05f933f36694fb44fe90ca4e73ec886.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\csharp</t>
-  </si>
-  <si>
-    <t>async.fb7e6562a96b068ce8f188a9a01a1a350b3786e2.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>csharp-6.f054f259d03c8f6ad7cfe33e83ae0905073abc73.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegate-class.04469eb80d6e6aac34f65fea453287188e1b66cd.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegates-events.13b9ae431dc65e962472a9f089cbc607444a0d11.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegates-overview.1032836974f9b23c8a790845708e68c7ac0dc8e3.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegates-patterns.b1cf7308c00cf85b704eceac928d65c7e05cb22b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegates-strongly-typed.49efe714f5cb0e4603fd3cf597d1b9072ef24ecf.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>distinguish-delegates-events.0b74be0746b04d724995663f41511b53c1d4f320.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>event-pattern.69c0983c2624f8e9ec96cde0ac1b457a7d345431.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>events-overview.6895286198c338fe5f27989a87bcbb3e51a642d7.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-classes.84f9c682074e9ad5b3718dd6c9133967b83fe7e2.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-building.4b597d1002b4396ecb33f06f4038cc77361ad2af.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-execution.a8b98bacf0a0bfe629117ad7acd6c10f2905b543.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-explained.062cd4b7229730802fad95bbc61398787daac4c4.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-interpreting.1327c85cae58c3091fe9fc6a1b10715a689ed97e.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-summary.201ee5f6028d637ae1aa2b18e61d2521c52a79f8.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees-translating.94b9bd5a171e1ce9852d2721f9e655d5394de549.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>expression-trees.b39d60187c732853fe485b97eac41692c8dd260c.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>implicitly-typed-lambda-expressions.60e7a9f683139131180bf8e2ae766488526091ca.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>indexers.6ee3f5f37dda8e514c40a01ebdc41e254b42f481.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>iterators.0df40ea5c68ac8561e5021c811e46e560573717c.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>modern-events.02c7181f2ca23448d3e8c68b8581108a34db8312.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>properties.51df8ec1803c024078778aa18555ebc8d5ee81d2.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\csharp\tutorials</t>
-  </si>
-  <si>
-    <t>console-teleprompter.12301eb0699d2d4b5fe67e8251d79b24baedc9ee.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>console-webapiclient.df7cf3ea50355e6f454d41cbd18e38d4003428bd.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.e6f14bd15d9ba180b914a2e448fc867ab3f8c918.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>microservices.429b8aaae4aa1be23a47ef5e3fdae81a433f6e6d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>working-with-linq.3aaea936956981bacf801f58a14b527f4ae692b6.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\fsharp</t>
-  </si>
-  <si>
-    <t>async.67a4c4cbce5eb33ce073e5fc5a9df5d06342e23b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>getting-started-netcore.ad81c83417296a1870ef09d6e056dc6d453f52b2.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.b0ceeb7aea312772827f7087f8a937edf1e7ed4d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\images</t>
-  </si>
-  <si>
-    <t>6ee6a35fa247dfe951f4df97818784b30600d543.png</t>
-  </si>
-  <si>
-    <t>docs\samples-and-tutorials</t>
-  </si>
-  <si>
-    <t>index.51c60a85ef778f387438df303e6ad9d2aa9ed3f3.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\standard</t>
-  </si>
-  <si>
-    <t>assembly-format.28db1c2eee4969148649923b2c83a0f9d8295d92.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>async-in-depth.16b4c489db1495cae0a0120c706ec82c79fdaad1.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>async.3c115f3a785660b634cfc3d7818885703e4965aa.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>class-libraries.7dadda8f3a69f2786b36b28fcabb59abbadd8677.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>clr.c6c600ab4fa351d3f792801bca39ed7a8c4d4965.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\standard\collections</t>
-  </si>
-  <si>
-    <t>commonly-used-collection-types.87b05596cbab370816c5e11832c8858aeaa2d9a1.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>comparisons-and-sorts-within-collections.a4814f345079fb61609f208213259d69dfd1affa.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>hashtable-and-dictionary-collection-types.726afc14b9c905ce623486d27942e828bf06348b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.3fe222dc280f54f96b43e0bc742c88c1b6de084a.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>selecting-a-collection-class.aa3adb37e1172576b891f4988de595d66a5011ba.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>sorted-collection-types.ae3aa45904d5407b15dfeb115fbc50a6f2dbaff5.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\standard\collections\threadsafe</t>
-  </si>
-  <si>
-    <t>blockingcollection-overview.47db7fe6b6dc98be9e5d8da6f1869eaa57afe519.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-add-and-remove-items.c77fbc4e7bd3b40ee1e7a82d6c35f6975e1ad92f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-add-and-take-items.74998e2a4567c4ce2e7e8cf4dd3bee2d71a5a9c8.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-add-bounding-and-blocking.d7e8e969f87f13bc8c0b4cb3105c65e5c49d1ed7.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-create-an-object-pool.67d4860ff587e91b4b30745bef2e52949e0b0972.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-use-arrays-of-blockingcollections.d399298da2f3e4c3dbeb438b63d75649f72fdc70.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>how-to-use-foreach-to-remove.5d91710e1ca1f740190d9df9b36fdcb019240590.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.71734fc8bf1ab51eccc74dd34d9e83715727c57b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>when-to-use-a-thread-safe-collection.c906ee56b8927c6037ad35092e542858518686e6.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>when-to-use-generic-collections.ec8a7ec4f16e4f7bd1072115323826242604a56b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>common-type-system.12e59626ca0328f39e75154d0bc212bcbae5a464.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>delegates-lambdas.71df54ba57d186484393e6e83b7a0dca5d9c3a97.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>exceptions.2c65f693d1e10768877aac0dd5db5448f6de5b33.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>framework-libraries.a910059a62e8080f3edc3e6a3141c5392e5f4840.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>frameworks.97b37c9150bfb4e97277c084ce00cbcace849bf8.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>gc-overview.09d3f3c36e4fb85bf89b55884bc8f58e8a4d5080.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>generics.1f8f95282e2b84cdfaeef3636a5944d55a152857.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.8bc2dd87c1d2edcd81672b92705979b37e524590.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>library.387c1e6b222531c2cedef18135a5fa775d5f0452.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>managed-code.c074f35f86522ea606301f15657bc0ee24da87df.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs\standard\media\assembly-format</t>
-  </si>
-  <si>
-    <t>938b47878d90fc32819bbfbae2b5737eab1bf677.png</t>
-  </si>
-  <si>
-    <t>docs\standard\media\portability-analyzer</t>
-  </si>
-  <si>
-    <t>878751ec4663e23a4ea7b70da29e750e222e19fa.png</t>
-  </si>
-  <si>
-    <t>f8208a75ae262d5130b5031bc8562d5b396442ef.png</t>
-  </si>
-  <si>
-    <t>31af85325450edc2abc7ba8dadf618272e81efc4.png</t>
-  </si>
-  <si>
-    <t>docs\standard\media\using-linq</t>
-  </si>
-  <si>
-    <t>e6b57c6b636d3d2d42299083d2b12eb049288e27.png</t>
-  </si>
-  <si>
-    <t>native-interop.8f6566123608155a52a2ab93eca340fe3087fb34.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>numerics.3cae565a7bf0ad930aed72b463f8dc1f484efead.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>portability-analyzer.e8a40fb40eb97b83690447183edbd03a56509a87.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>using-linq.9202ee2cc6a78e5d44a90dd7b156929a14f8fd86.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>docs</t>
-  </si>
-  <si>
-    <t>welcome.cf84032b4d2e283cbf5c69d78077d1efb10a3c58.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>index.b8d322cca13b7303167b216a3efe71db4e1687a1.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>README.8ec9a00bfd09b3190ac6b22251dbb1aa95a0579d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\console-apps\Fibonacci</t>
-  </si>
-  <si>
-    <t>README.833d3889a48c2604c718bd6cb2dd4b40fb611c09.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\console-apps\FibonacciBetter</t>
-  </si>
-  <si>
-    <t>README.aaf05806fc8bf002d3b366347ba2bd058b82f9b4.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\console-apps\Hello</t>
-  </si>
-  <si>
-    <t>README.2e42c2d62eea4c136751e34541c15ccf9f5a1c2a.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\console-apps\HelloNative</t>
-  </si>
-  <si>
-    <t>README.90878ce4606d18256fdb51ddec9bf70aacfd2fa0.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\console-apps\NewTypes</t>
-  </si>
-  <si>
-    <t>README.a258da1a8e58fc590c32169dad125de335dae304.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\core-projects\libraries</t>
-  </si>
-  <si>
-    <t>README.6deb49b78f2b185dfd36ec0d5e01934d48f66291.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\console-linq</t>
-  </si>
-  <si>
-    <t>README.c1fd3bff6fb8364413ed8f7d51aa552039a25f54.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\console-teleprompter</t>
-  </si>
-  <si>
-    <t>README.b0addf503313b1a99b89254739f8e53852a496e7.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\console-webapiclient</t>
-  </si>
-  <si>
-    <t>README.f3964029da15b075c1a5d79797051a6a2449182d.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\delegates-and-events</t>
-  </si>
-  <si>
-    <t>README.ce0f559e48855520c3e9f6e7f72367231da58b98.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\events</t>
-  </si>
-  <si>
-    <t>README.6efcda3e0b4b04ebc8e2ba8994a543ed0de3356b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\expression-trees</t>
-  </si>
-  <si>
-    <t>README.065c32729da82224a977901d6700fd9f24c159e5.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\indexers</t>
-  </si>
-  <si>
-    <t>README.7ed44e9c8a8d9ca22334b381fd1c40c0880c277b.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\iterators</t>
-  </si>
-  <si>
-    <t>README.5d6c14b3c88e47cf1a390ba2348181637977f186.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\WeatherMicroservice</t>
-  </si>
-  <si>
-    <t>README.6bb043903290a12848181c19f62ec3d21c50140f.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\csharp-language\WeatherMicroservice\wwwroot</t>
-  </si>
-  <si>
-    <t>README.bf3e5645731a4878d9c02fdb008220f45c975f97.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\getting-started\golden</t>
-  </si>
-  <si>
-    <t>README.2cf499dfab094d02d0501c30d2e74e7d1bd21d8a.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\linq\csharp</t>
-  </si>
-  <si>
-    <t>README.67e561b1f112389541ad29652f348dc14d2e4ecc.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples</t>
-  </si>
-  <si>
-    <t>README.ed595a0cdde816cbf12782578f6938544d11577a.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>samples\unit-testing\using-dotnet-test</t>
-  </si>
-  <si>
-    <t>README.c70fdc64850f508e9bf8e2cfd52489f8becd9845.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>styleguide</t>
-  </si>
-  <si>
-    <t>template.f8ef37f92e542c373ce9d5385182d53bb1ce5a60.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>voice-tone.1d6a374e632fbd93441b10f49206a284752ca333.zh-cn.xlf</t>
-  </si>
-  <si>
-    <t>TOC.c5e56b4d05e38e466c0192461b6c26065f810c46.zh-cn.xlf</t>
   </si>
   <si>
     <t>Invalid character (���) in string: Also, remove the "wrench" icon (🔧) from the TOC and the file heading, if applicable. at index 32</t>
@@ -1812,7 +1815,7 @@
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="12.1930160522461" customWidth="1"/>
     <col min="4" max="4" width="13.9639423915318" customWidth="1"/>
-    <col min="5" max="5" width="23.1374904087612" customWidth="1"/>
+    <col min="5" max="5" width="29.9777047293527" customWidth="1"/>
     <col min="6" max="6" width="29.5073743547712" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5552,14 +5555,14 @@
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="15.7369144984654" customWidth="1"/>
-    <col min="3" max="3" width="23.1374904087612" customWidth="1"/>
+    <col min="3" max="3" width="29.9777047293527" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="10.1100556509835" customWidth="1"/>
     <col min="6" max="6" width="19.556018284389" customWidth="1"/>
     <col min="7" max="7" width="40" customWidth="1"/>
     <col min="8" max="8" width="25.2197069440569" customWidth="1"/>
-    <col min="9" max="9" width="18.6506053379604" customWidth="1"/>
-    <col min="10" max="10" width="21.7054770333426" customWidth="1"/>
+    <col min="9" max="9" width="40" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
     <col min="11" max="11" width="27.1533006940569" customWidth="1"/>
     <col min="12" max="12" width="19.298205784389" customWidth="1"/>
     <col min="13" max="13" width="17.7080830165318" customWidth="1"/>
@@ -5643,11 +5646,11 @@
       <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>9</v>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>9</v>
+        <v>338</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>339</v>
@@ -5693,11 +5696,11 @@
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>9</v>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>9</v>
+        <v>341</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>339</v>
@@ -5743,11 +5746,11 @@
       <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>9</v>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>9</v>
+        <v>343</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>339</v>
@@ -5793,11 +5796,11 @@
       <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="0" t="s">
-        <v>9</v>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>9</v>
+        <v>345</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>339</v>
@@ -5843,11 +5846,11 @@
       <c r="H6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>9</v>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>339</v>
@@ -5893,11 +5896,11 @@
       <c r="H7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="0" t="s">
-        <v>9</v>
+      <c r="I7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>9</v>
+        <v>348</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>339</v>
@@ -5943,11 +5946,11 @@
       <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>9</v>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>9</v>
+        <v>350</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>339</v>
@@ -5993,11 +5996,11 @@
       <c r="H9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>9</v>
+      <c r="I9" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>9</v>
+        <v>352</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>339</v>
@@ -6043,11 +6046,11 @@
       <c r="H10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>9</v>
+      <c r="I10" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>9</v>
+        <v>353</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>339</v>
@@ -6093,11 +6096,11 @@
       <c r="H11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="0" t="s">
-        <v>9</v>
+      <c r="I11" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>9</v>
+        <v>354</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>339</v>
@@ -6143,11 +6146,11 @@
       <c r="H12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>9</v>
+      <c r="I12" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>9</v>
+        <v>355</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>339</v>
@@ -6193,11 +6196,11 @@
       <c r="H13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>9</v>
+      <c r="I13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>9</v>
+        <v>356</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>339</v>
@@ -6243,11 +6246,11 @@
       <c r="H14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>9</v>
+      <c r="I14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>9</v>
+        <v>358</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>339</v>
@@ -6293,11 +6296,11 @@
       <c r="H15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="0" t="s">
-        <v>9</v>
+      <c r="I15" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>9</v>
+        <v>360</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>339</v>
@@ -6343,11 +6346,11 @@
       <c r="H16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>9</v>
+      <c r="I16" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>9</v>
+        <v>361</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>339</v>
@@ -6393,11 +6396,11 @@
       <c r="H17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>9</v>
+      <c r="I17" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>9</v>
+        <v>363</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>339</v>
@@ -6443,11 +6446,11 @@
       <c r="H18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>9</v>
+      <c r="I18" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>9</v>
+        <v>364</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>339</v>
@@ -6493,11 +6496,11 @@
       <c r="H19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>9</v>
+      <c r="I19" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>9</v>
+        <v>366</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>339</v>
@@ -6543,11 +6546,11 @@
       <c r="H20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="0" t="s">
-        <v>9</v>
+      <c r="I20" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>9</v>
+        <v>367</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>339</v>
@@ -6593,11 +6596,11 @@
       <c r="H21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="0" t="s">
-        <v>9</v>
+      <c r="I21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>9</v>
+        <v>368</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>339</v>
@@ -6643,11 +6646,11 @@
       <c r="H22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>9</v>
+      <c r="I22" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>9</v>
+        <v>369</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>339</v>
@@ -6693,11 +6696,11 @@
       <c r="H23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>9</v>
+      <c r="I23" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>9</v>
+        <v>370</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>339</v>
@@ -6743,11 +6746,11 @@
       <c r="H24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="0" t="s">
-        <v>9</v>
+      <c r="I24" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>9</v>
+        <v>371</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>339</v>
@@ -6793,11 +6796,11 @@
       <c r="H25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>9</v>
+      <c r="I25" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>9</v>
+        <v>372</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>339</v>
@@ -6843,11 +6846,11 @@
       <c r="H26" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="0" t="s">
-        <v>9</v>
+      <c r="I26" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>9</v>
+        <v>373</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>339</v>
@@ -6893,11 +6896,11 @@
       <c r="H27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="0" t="s">
-        <v>9</v>
+      <c r="I27" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>9</v>
+        <v>375</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>339</v>
@@ -6943,11 +6946,11 @@
       <c r="H28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="0" t="s">
-        <v>9</v>
+      <c r="I28" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>9</v>
+        <v>376</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>339</v>
@@ -6993,11 +6996,11 @@
       <c r="H29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="0" t="s">
-        <v>9</v>
+      <c r="I29" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>9</v>
+        <v>378</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>339</v>
@@ -7043,11 +7046,11 @@
       <c r="H30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="0" t="s">
-        <v>9</v>
+      <c r="I30" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>9</v>
+        <v>379</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>339</v>
@@ -7093,11 +7096,11 @@
       <c r="H31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>9</v>
+      <c r="I31" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>9</v>
+        <v>380</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>339</v>
@@ -7143,11 +7146,11 @@
       <c r="H32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>9</v>
+      <c r="I32" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>9</v>
+        <v>381</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>339</v>
@@ -7193,11 +7196,11 @@
       <c r="H33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I33" s="0" t="s">
-        <v>9</v>
+      <c r="I33" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>9</v>
+        <v>382</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>339</v>
@@ -7243,11 +7246,11 @@
       <c r="H34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>9</v>
+      <c r="I34" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>9</v>
+        <v>383</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>339</v>
@@ -7293,11 +7296,11 @@
       <c r="H35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="0" t="s">
-        <v>9</v>
+      <c r="I35" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>9</v>
+        <v>384</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>339</v>
@@ -7343,11 +7346,11 @@
       <c r="H36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I36" s="0" t="s">
-        <v>9</v>
+      <c r="I36" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>9</v>
+        <v>385</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>339</v>
@@ -7393,11 +7396,11 @@
       <c r="H37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="0" t="s">
-        <v>9</v>
+      <c r="I37" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>9</v>
+        <v>386</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>339</v>
@@ -7443,11 +7446,11 @@
       <c r="H38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="0" t="s">
-        <v>9</v>
+      <c r="I38" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>9</v>
+        <v>387</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>339</v>
@@ -7493,11 +7496,11 @@
       <c r="H39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I39" s="0" t="s">
-        <v>9</v>
+      <c r="I39" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>9</v>
+        <v>388</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>339</v>
@@ -7543,11 +7546,11 @@
       <c r="H40" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="0" t="s">
-        <v>9</v>
+      <c r="I40" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>9</v>
+        <v>389</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>339</v>
@@ -7593,11 +7596,11 @@
       <c r="H41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="0" t="s">
-        <v>9</v>
+      <c r="I41" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>9</v>
+        <v>391</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>339</v>
@@ -7643,11 +7646,11 @@
       <c r="H42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I42" s="0" t="s">
-        <v>9</v>
+      <c r="I42" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>9</v>
+        <v>392</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>339</v>
@@ -7693,11 +7696,11 @@
       <c r="H43" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I43" s="0" t="s">
-        <v>9</v>
+      <c r="I43" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>9</v>
+        <v>393</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>339</v>
@@ -7743,11 +7746,11 @@
       <c r="H44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I44" s="0" t="s">
-        <v>9</v>
+      <c r="I44" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>9</v>
+        <v>394</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>339</v>
@@ -7793,11 +7796,11 @@
       <c r="H45" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I45" s="0" t="s">
-        <v>9</v>
+      <c r="I45" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>9</v>
+        <v>395</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>339</v>
@@ -7843,11 +7846,11 @@
       <c r="H46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="0" t="s">
-        <v>9</v>
+      <c r="I46" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>9</v>
+        <v>396</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>339</v>
@@ -7893,11 +7896,11 @@
       <c r="H47" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="0" t="s">
-        <v>9</v>
+      <c r="I47" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>9</v>
+        <v>398</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>339</v>
@@ -7943,11 +7946,11 @@
       <c r="H48" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="0" t="s">
-        <v>9</v>
+      <c r="I48" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>9</v>
+        <v>399</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>339</v>
@@ -7993,11 +7996,11 @@
       <c r="H49" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I49" s="0" t="s">
-        <v>9</v>
+      <c r="I49" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>9</v>
+        <v>400</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>339</v>
@@ -8043,11 +8046,11 @@
       <c r="H50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I50" s="0" t="s">
-        <v>9</v>
+      <c r="I50" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>9</v>
+        <v>401</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>339</v>
@@ -8093,11 +8096,11 @@
       <c r="H51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="0" t="s">
-        <v>9</v>
+      <c r="I51" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>9</v>
+        <v>403</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>339</v>
@@ -8143,11 +8146,11 @@
       <c r="H52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="0" t="s">
-        <v>9</v>
+      <c r="I52" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>9</v>
+        <v>404</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>339</v>
@@ -8193,11 +8196,11 @@
       <c r="H53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I53" s="0" t="s">
-        <v>9</v>
+      <c r="I53" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>9</v>
+        <v>406</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>339</v>
@@ -8243,11 +8246,11 @@
       <c r="H54" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I54" s="0" t="s">
-        <v>9</v>
+      <c r="I54" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>9</v>
+        <v>407</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>339</v>
@@ -8293,11 +8296,11 @@
       <c r="H55" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I55" s="0" t="s">
-        <v>9</v>
+      <c r="I55" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>9</v>
+        <v>408</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>339</v>
@@ -8343,11 +8346,11 @@
       <c r="H56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I56" s="0" t="s">
-        <v>9</v>
+      <c r="I56" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>9</v>
+        <v>409</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>339</v>
@@ -8393,11 +8396,11 @@
       <c r="H57" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I57" s="0" t="s">
-        <v>9</v>
+      <c r="I57" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>9</v>
+        <v>410</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>339</v>
@@ -8443,11 +8446,11 @@
       <c r="H58" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I58" s="0" t="s">
-        <v>9</v>
+      <c r="I58" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>9</v>
+        <v>412</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>339</v>
@@ -8493,11 +8496,11 @@
       <c r="H59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I59" s="0" t="s">
-        <v>9</v>
+      <c r="I59" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>9</v>
+        <v>413</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>339</v>
@@ -8543,11 +8546,11 @@
       <c r="H60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I60" s="0" t="s">
-        <v>9</v>
+      <c r="I60" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>9</v>
+        <v>415</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>339</v>
@@ -8593,11 +8596,11 @@
       <c r="H61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I61" s="0" t="s">
-        <v>9</v>
+      <c r="I61" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="J61" s="0" t="s">
-        <v>9</v>
+        <v>416</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>339</v>
@@ -8643,11 +8646,11 @@
       <c r="H62" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I62" s="0" t="s">
-        <v>9</v>
+      <c r="I62" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>9</v>
+        <v>417</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>339</v>
@@ -8693,11 +8696,11 @@
       <c r="H63" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I63" s="0" t="s">
-        <v>9</v>
+      <c r="I63" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>9</v>
+        <v>418</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>339</v>
@@ -8743,11 +8746,11 @@
       <c r="H64" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I64" s="0" t="s">
-        <v>9</v>
+      <c r="I64" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>9</v>
+        <v>419</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>339</v>
@@ -8793,11 +8796,11 @@
       <c r="H65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I65" s="0" t="s">
-        <v>9</v>
+      <c r="I65" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>9</v>
+        <v>420</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>339</v>
@@ -8843,11 +8846,11 @@
       <c r="H66" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I66" s="0" t="s">
-        <v>9</v>
+      <c r="I66" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>9</v>
+        <v>421</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>339</v>
@@ -8893,11 +8896,11 @@
       <c r="H67" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I67" s="0" t="s">
-        <v>9</v>
+      <c r="I67" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>9</v>
+        <v>422</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>339</v>
@@ -8943,11 +8946,11 @@
       <c r="H68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I68" s="0" t="s">
-        <v>9</v>
+      <c r="I68" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>9</v>
+        <v>423</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>339</v>
@@ -8993,11 +8996,11 @@
       <c r="H69" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="0" t="s">
-        <v>9</v>
+      <c r="I69" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>9</v>
+        <v>424</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>339</v>
@@ -9043,11 +9046,11 @@
       <c r="H70" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I70" s="0" t="s">
-        <v>9</v>
+      <c r="I70" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>9</v>
+        <v>425</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>339</v>
@@ -9093,11 +9096,11 @@
       <c r="H71" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I71" s="0" t="s">
-        <v>9</v>
+      <c r="I71" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>9</v>
+        <v>426</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>339</v>
@@ -9143,11 +9146,11 @@
       <c r="H72" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I72" s="0" t="s">
-        <v>9</v>
+      <c r="I72" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>9</v>
+        <v>427</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>339</v>
@@ -9193,11 +9196,11 @@
       <c r="H73" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I73" s="0" t="s">
-        <v>9</v>
+      <c r="I73" s="1" t="s">
+        <v>144</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>9</v>
+        <v>428</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>339</v>
@@ -9243,11 +9246,11 @@
       <c r="H74" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I74" s="0" t="s">
-        <v>9</v>
+      <c r="I74" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>9</v>
+        <v>429</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>339</v>
@@ -9293,11 +9296,11 @@
       <c r="H75" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I75" s="0" t="s">
-        <v>9</v>
+      <c r="I75" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>9</v>
+        <v>430</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>339</v>
@@ -9343,11 +9346,11 @@
       <c r="H76" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I76" s="0" t="s">
-        <v>9</v>
+      <c r="I76" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>9</v>
+        <v>431</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>339</v>
@@ -9393,11 +9396,11 @@
       <c r="H77" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I77" s="0" t="s">
-        <v>9</v>
+      <c r="I77" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>9</v>
+        <v>432</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>339</v>
@@ -9443,11 +9446,11 @@
       <c r="H78" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I78" s="0" t="s">
-        <v>9</v>
+      <c r="I78" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>9</v>
+        <v>433</v>
       </c>
       <c r="K78" s="2" t="s">
         <v>339</v>
@@ -9493,11 +9496,11 @@
       <c r="H79" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I79" s="0" t="s">
-        <v>9</v>
+      <c r="I79" s="1" t="s">
+        <v>156</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>9</v>
+        <v>434</v>
       </c>
       <c r="K79" s="2" t="s">
         <v>339</v>
@@ -9543,11 +9546,11 @@
       <c r="H80" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I80" s="0" t="s">
-        <v>9</v>
+      <c r="I80" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>9</v>
+        <v>435</v>
       </c>
       <c r="K80" s="2" t="s">
         <v>339</v>
@@ -9593,11 +9596,11 @@
       <c r="H81" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I81" s="0" t="s">
-        <v>9</v>
+      <c r="I81" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>9</v>
+        <v>436</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>339</v>
@@ -9643,11 +9646,11 @@
       <c r="H82" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I82" s="0" t="s">
-        <v>9</v>
+      <c r="I82" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>9</v>
+        <v>437</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>339</v>
@@ -9693,11 +9696,11 @@
       <c r="H83" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I83" s="0" t="s">
-        <v>9</v>
+      <c r="I83" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="J83" s="0" t="s">
-        <v>9</v>
+        <v>439</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>339</v>
@@ -9743,11 +9746,11 @@
       <c r="H84" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I84" s="0" t="s">
-        <v>9</v>
+      <c r="I84" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="J84" s="0" t="s">
-        <v>9</v>
+        <v>440</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>339</v>
@@ -9793,11 +9796,11 @@
       <c r="H85" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I85" s="0" t="s">
-        <v>9</v>
+      <c r="I85" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>9</v>
+        <v>441</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>339</v>
@@ -9843,11 +9846,11 @@
       <c r="H86" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I86" s="0" t="s">
-        <v>9</v>
+      <c r="I86" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="J86" s="0" t="s">
-        <v>9</v>
+        <v>442</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>339</v>
@@ -9893,11 +9896,11 @@
       <c r="H87" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I87" s="0" t="s">
-        <v>9</v>
+      <c r="I87" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="J87" s="0" t="s">
-        <v>9</v>
+        <v>443</v>
       </c>
       <c r="K87" s="2" t="s">
         <v>339</v>
@@ -9943,11 +9946,11 @@
       <c r="H88" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I88" s="0" t="s">
-        <v>9</v>
+      <c r="I88" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>9</v>
+        <v>445</v>
       </c>
       <c r="K88" s="2" t="s">
         <v>339</v>
@@ -9993,11 +9996,11 @@
       <c r="H89" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I89" s="0" t="s">
-        <v>9</v>
+      <c r="I89" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>9</v>
+        <v>446</v>
       </c>
       <c r="K89" s="2" t="s">
         <v>339</v>
@@ -10043,11 +10046,11 @@
       <c r="H90" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I90" s="0" t="s">
-        <v>9</v>
+      <c r="I90" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>9</v>
+        <v>447</v>
       </c>
       <c r="K90" s="2" t="s">
         <v>339</v>
@@ -10093,11 +10096,11 @@
       <c r="H91" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I91" s="0" t="s">
-        <v>9</v>
+      <c r="I91" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="J91" s="0" t="s">
-        <v>9</v>
+        <v>449</v>
       </c>
       <c r="K91" s="2" t="s">
         <v>339</v>
@@ -10143,11 +10146,11 @@
       <c r="H92" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I92" s="0" t="s">
-        <v>9</v>
+      <c r="I92" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>9</v>
+        <v>451</v>
       </c>
       <c r="K92" s="2" t="s">
         <v>339</v>
@@ -10193,11 +10196,11 @@
       <c r="H93" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I93" s="0" t="s">
-        <v>9</v>
+      <c r="I93" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>9</v>
+        <v>453</v>
       </c>
       <c r="K93" s="2" t="s">
         <v>339</v>
@@ -10243,11 +10246,11 @@
       <c r="H94" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I94" s="0" t="s">
-        <v>9</v>
+      <c r="I94" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>9</v>
+        <v>454</v>
       </c>
       <c r="K94" s="2" t="s">
         <v>339</v>
@@ -10293,11 +10296,11 @@
       <c r="H95" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I95" s="0" t="s">
-        <v>9</v>
+      <c r="I95" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>9</v>
+        <v>455</v>
       </c>
       <c r="K95" s="2" t="s">
         <v>339</v>
@@ -10343,11 +10346,11 @@
       <c r="H96" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I96" s="0" t="s">
-        <v>9</v>
+      <c r="I96" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>9</v>
+        <v>456</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>339</v>
@@ -10393,11 +10396,11 @@
       <c r="H97" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I97" s="0" t="s">
-        <v>9</v>
+      <c r="I97" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>9</v>
+        <v>457</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>339</v>
@@ -10443,11 +10446,11 @@
       <c r="H98" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I98" s="0" t="s">
-        <v>9</v>
+      <c r="I98" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>9</v>
+        <v>459</v>
       </c>
       <c r="K98" s="2" t="s">
         <v>339</v>
@@ -10493,11 +10496,11 @@
       <c r="H99" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I99" s="0" t="s">
-        <v>9</v>
+      <c r="I99" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>9</v>
+        <v>460</v>
       </c>
       <c r="K99" s="2" t="s">
         <v>339</v>
@@ -10543,11 +10546,11 @@
       <c r="H100" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I100" s="0" t="s">
-        <v>9</v>
+      <c r="I100" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>9</v>
+        <v>461</v>
       </c>
       <c r="K100" s="2" t="s">
         <v>339</v>
@@ -10593,11 +10596,11 @@
       <c r="H101" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I101" s="0" t="s">
-        <v>9</v>
+      <c r="I101" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>9</v>
+        <v>462</v>
       </c>
       <c r="K101" s="2" t="s">
         <v>339</v>
@@ -10643,11 +10646,11 @@
       <c r="H102" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I102" s="0" t="s">
-        <v>9</v>
+      <c r="I102" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>9</v>
+        <v>463</v>
       </c>
       <c r="K102" s="2" t="s">
         <v>339</v>
@@ -10693,11 +10696,11 @@
       <c r="H103" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I103" s="0" t="s">
-        <v>9</v>
+      <c r="I103" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>9</v>
+        <v>464</v>
       </c>
       <c r="K103" s="2" t="s">
         <v>339</v>
@@ -10743,11 +10746,11 @@
       <c r="H104" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I104" s="0" t="s">
-        <v>9</v>
+      <c r="I104" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="J104" s="0" t="s">
-        <v>9</v>
+        <v>466</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>339</v>
@@ -10793,11 +10796,11 @@
       <c r="H105" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I105" s="0" t="s">
-        <v>9</v>
+      <c r="I105" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="J105" s="0" t="s">
-        <v>9</v>
+        <v>467</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>339</v>
@@ -10843,11 +10846,11 @@
       <c r="H106" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I106" s="0" t="s">
-        <v>9</v>
+      <c r="I106" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="J106" s="0" t="s">
-        <v>9</v>
+        <v>468</v>
       </c>
       <c r="K106" s="2" t="s">
         <v>339</v>
@@ -10893,11 +10896,11 @@
       <c r="H107" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I107" s="0" t="s">
-        <v>9</v>
+      <c r="I107" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="J107" s="0" t="s">
-        <v>9</v>
+        <v>469</v>
       </c>
       <c r="K107" s="2" t="s">
         <v>339</v>
@@ -10943,11 +10946,11 @@
       <c r="H108" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I108" s="0" t="s">
-        <v>9</v>
+      <c r="I108" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="J108" s="0" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>339</v>
@@ -10993,11 +10996,11 @@
       <c r="H109" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I109" s="0" t="s">
-        <v>9</v>
+      <c r="I109" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="J109" s="0" t="s">
-        <v>9</v>
+        <v>471</v>
       </c>
       <c r="K109" s="2" t="s">
         <v>339</v>
@@ -11043,11 +11046,11 @@
       <c r="H110" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I110" s="0" t="s">
-        <v>9</v>
+      <c r="I110" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="J110" s="0" t="s">
-        <v>9</v>
+        <v>472</v>
       </c>
       <c r="K110" s="2" t="s">
         <v>339</v>
@@ -11093,11 +11096,11 @@
       <c r="H111" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I111" s="0" t="s">
-        <v>9</v>
+      <c r="I111" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>9</v>
+        <v>473</v>
       </c>
       <c r="K111" s="2" t="s">
         <v>339</v>
@@ -11143,11 +11146,11 @@
       <c r="H112" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I112" s="0" t="s">
-        <v>9</v>
+      <c r="I112" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="J112" s="0" t="s">
-        <v>9</v>
+        <v>474</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>339</v>
@@ -11193,11 +11196,11 @@
       <c r="H113" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I113" s="0" t="s">
-        <v>9</v>
+      <c r="I113" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="J113" s="0" t="s">
-        <v>9</v>
+        <v>475</v>
       </c>
       <c r="K113" s="2" t="s">
         <v>339</v>
@@ -11243,11 +11246,11 @@
       <c r="H114" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I114" s="0" t="s">
-        <v>9</v>
+      <c r="I114" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="J114" s="0" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="K114" s="2" t="s">
         <v>339</v>
@@ -11293,11 +11296,11 @@
       <c r="H115" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I115" s="0" t="s">
-        <v>9</v>
+      <c r="I115" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="J115" s="0" t="s">
-        <v>9</v>
+        <v>477</v>
       </c>
       <c r="K115" s="2" t="s">
         <v>339</v>
@@ -11343,11 +11346,11 @@
       <c r="H116" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I116" s="0" t="s">
-        <v>9</v>
+      <c r="I116" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="J116" s="0" t="s">
-        <v>9</v>
+        <v>478</v>
       </c>
       <c r="K116" s="2" t="s">
         <v>339</v>
@@ -11393,11 +11396,11 @@
       <c r="H117" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I117" s="0" t="s">
-        <v>9</v>
+      <c r="I117" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>9</v>
+        <v>479</v>
       </c>
       <c r="K117" s="2" t="s">
         <v>339</v>
@@ -11443,11 +11446,11 @@
       <c r="H118" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I118" s="0" t="s">
-        <v>9</v>
+      <c r="I118" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="J118" s="0" t="s">
-        <v>9</v>
+        <v>480</v>
       </c>
       <c r="K118" s="2" t="s">
         <v>339</v>
@@ -11493,11 +11496,11 @@
       <c r="H119" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I119" s="0" t="s">
-        <v>9</v>
+      <c r="I119" s="1" t="s">
+        <v>229</v>
       </c>
       <c r="J119" s="0" t="s">
-        <v>9</v>
+        <v>481</v>
       </c>
       <c r="K119" s="2" t="s">
         <v>339</v>
@@ -11543,11 +11546,11 @@
       <c r="H120" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I120" s="0" t="s">
-        <v>9</v>
+      <c r="I120" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="J120" s="0" t="s">
-        <v>9</v>
+        <v>482</v>
       </c>
       <c r="K120" s="2" t="s">
         <v>339</v>
@@ -11593,11 +11596,11 @@
       <c r="H121" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I121" s="0" t="s">
-        <v>9</v>
+      <c r="I121" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J121" s="0" t="s">
-        <v>9</v>
+        <v>483</v>
       </c>
       <c r="K121" s="2" t="s">
         <v>339</v>
@@ -11643,11 +11646,11 @@
       <c r="H122" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I122" s="0" t="s">
-        <v>9</v>
+      <c r="I122" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="J122" s="0" t="s">
-        <v>9</v>
+        <v>484</v>
       </c>
       <c r="K122" s="2" t="s">
         <v>339</v>
@@ -11693,11 +11696,11 @@
       <c r="H123" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I123" s="0" t="s">
-        <v>9</v>
+      <c r="I123" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="J123" s="0" t="s">
-        <v>9</v>
+        <v>485</v>
       </c>
       <c r="K123" s="2" t="s">
         <v>339</v>
@@ -11743,11 +11746,11 @@
       <c r="H124" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I124" s="0" t="s">
-        <v>9</v>
+      <c r="I124" s="1" t="s">
+        <v>238</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>9</v>
+        <v>487</v>
       </c>
       <c r="K124" s="2" t="s">
         <v>339</v>
@@ -11793,11 +11796,11 @@
       <c r="H125" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I125" s="0" t="s">
-        <v>9</v>
+      <c r="I125" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="J125" s="0" t="s">
-        <v>9</v>
+        <v>489</v>
       </c>
       <c r="K125" s="2" t="s">
         <v>339</v>
@@ -11843,11 +11846,11 @@
       <c r="H126" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I126" s="0" t="s">
-        <v>9</v>
+      <c r="I126" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="J126" s="0" t="s">
-        <v>9</v>
+        <v>490</v>
       </c>
       <c r="K126" s="2" t="s">
         <v>339</v>
@@ -11893,11 +11896,11 @@
       <c r="H127" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I127" s="0" t="s">
-        <v>9</v>
+      <c r="I127" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="J127" s="0" t="s">
-        <v>9</v>
+        <v>491</v>
       </c>
       <c r="K127" s="2" t="s">
         <v>339</v>
@@ -11943,11 +11946,11 @@
       <c r="H128" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I128" s="0" t="s">
-        <v>9</v>
+      <c r="I128" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="J128" s="0" t="s">
-        <v>9</v>
+        <v>493</v>
       </c>
       <c r="K128" s="2" t="s">
         <v>339</v>
@@ -11993,11 +11996,11 @@
       <c r="H129" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I129" s="0" t="s">
-        <v>9</v>
+      <c r="I129" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="J129" s="0" t="s">
-        <v>9</v>
+        <v>494</v>
       </c>
       <c r="K129" s="2" t="s">
         <v>339</v>
@@ -12043,11 +12046,11 @@
       <c r="H130" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I130" s="0" t="s">
-        <v>9</v>
+      <c r="I130" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="J130" s="0" t="s">
-        <v>9</v>
+        <v>495</v>
       </c>
       <c r="K130" s="2" t="s">
         <v>339</v>
@@ -12093,11 +12096,11 @@
       <c r="H131" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I131" s="0" t="s">
-        <v>9</v>
+      <c r="I131" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="J131" s="0" t="s">
-        <v>9</v>
+        <v>496</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>339</v>
@@ -12143,11 +12146,11 @@
       <c r="H132" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I132" s="0" t="s">
-        <v>9</v>
+      <c r="I132" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="J132" s="0" t="s">
-        <v>9</v>
+        <v>497</v>
       </c>
       <c r="K132" s="2" t="s">
         <v>339</v>
@@ -12193,11 +12196,11 @@
       <c r="H133" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I133" s="0" t="s">
-        <v>9</v>
+      <c r="I133" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="J133" s="0" t="s">
-        <v>9</v>
+        <v>499</v>
       </c>
       <c r="K133" s="2" t="s">
         <v>339</v>
@@ -12243,11 +12246,11 @@
       <c r="H134" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I134" s="0" t="s">
-        <v>9</v>
+      <c r="I134" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="J134" s="0" t="s">
-        <v>9</v>
+        <v>500</v>
       </c>
       <c r="K134" s="2" t="s">
         <v>339</v>
@@ -12293,11 +12296,11 @@
       <c r="H135" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I135" s="0" t="s">
-        <v>9</v>
+      <c r="I135" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J135" s="0" t="s">
-        <v>9</v>
+        <v>501</v>
       </c>
       <c r="K135" s="2" t="s">
         <v>339</v>
@@ -12343,11 +12346,11 @@
       <c r="H136" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I136" s="0" t="s">
-        <v>9</v>
+      <c r="I136" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J136" s="0" t="s">
-        <v>9</v>
+        <v>503</v>
       </c>
       <c r="K136" s="2" t="s">
         <v>339</v>
@@ -12393,11 +12396,11 @@
       <c r="H137" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I137" s="0" t="s">
-        <v>9</v>
+      <c r="I137" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J137" s="0" t="s">
-        <v>9</v>
+        <v>505</v>
       </c>
       <c r="K137" s="2" t="s">
         <v>339</v>
@@ -12443,11 +12446,11 @@
       <c r="H138" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I138" s="0" t="s">
-        <v>9</v>
+      <c r="I138" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J138" s="0" t="s">
-        <v>9</v>
+        <v>507</v>
       </c>
       <c r="K138" s="2" t="s">
         <v>339</v>
@@ -12493,11 +12496,11 @@
       <c r="H139" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I139" s="0" t="s">
-        <v>9</v>
+      <c r="I139" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J139" s="0" t="s">
-        <v>9</v>
+        <v>509</v>
       </c>
       <c r="K139" s="2" t="s">
         <v>339</v>
@@ -12543,11 +12546,11 @@
       <c r="H140" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I140" s="0" t="s">
-        <v>9</v>
+      <c r="I140" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J140" s="0" t="s">
-        <v>9</v>
+        <v>511</v>
       </c>
       <c r="K140" s="2" t="s">
         <v>339</v>
@@ -12593,11 +12596,11 @@
       <c r="H141" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I141" s="0" t="s">
-        <v>9</v>
+      <c r="I141" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J141" s="0" t="s">
-        <v>9</v>
+        <v>513</v>
       </c>
       <c r="K141" s="2" t="s">
         <v>339</v>
@@ -12643,11 +12646,11 @@
       <c r="H142" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I142" s="0" t="s">
-        <v>9</v>
+      <c r="I142" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J142" s="0" t="s">
-        <v>9</v>
+        <v>515</v>
       </c>
       <c r="K142" s="2" t="s">
         <v>339</v>
@@ -12693,11 +12696,11 @@
       <c r="H143" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I143" s="0" t="s">
-        <v>9</v>
+      <c r="I143" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J143" s="0" t="s">
-        <v>9</v>
+        <v>517</v>
       </c>
       <c r="K143" s="2" t="s">
         <v>339</v>
@@ -12743,11 +12746,11 @@
       <c r="H144" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I144" s="0" t="s">
-        <v>9</v>
+      <c r="I144" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J144" s="0" t="s">
-        <v>9</v>
+        <v>519</v>
       </c>
       <c r="K144" s="2" t="s">
         <v>339</v>
@@ -12793,11 +12796,11 @@
       <c r="H145" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I145" s="0" t="s">
-        <v>9</v>
+      <c r="I145" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J145" s="0" t="s">
-        <v>9</v>
+        <v>521</v>
       </c>
       <c r="K145" s="2" t="s">
         <v>339</v>
@@ -12843,11 +12846,11 @@
       <c r="H146" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I146" s="0" t="s">
-        <v>9</v>
+      <c r="I146" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J146" s="0" t="s">
-        <v>9</v>
+        <v>523</v>
       </c>
       <c r="K146" s="2" t="s">
         <v>339</v>
@@ -12893,11 +12896,11 @@
       <c r="H147" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I147" s="0" t="s">
-        <v>9</v>
+      <c r="I147" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J147" s="0" t="s">
-        <v>9</v>
+        <v>525</v>
       </c>
       <c r="K147" s="2" t="s">
         <v>339</v>
@@ -12943,11 +12946,11 @@
       <c r="H148" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I148" s="0" t="s">
-        <v>9</v>
+      <c r="I148" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J148" s="0" t="s">
-        <v>9</v>
+        <v>527</v>
       </c>
       <c r="K148" s="2" t="s">
         <v>339</v>
@@ -12993,11 +12996,11 @@
       <c r="H149" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I149" s="0" t="s">
-        <v>9</v>
+      <c r="I149" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J149" s="0" t="s">
-        <v>9</v>
+        <v>529</v>
       </c>
       <c r="K149" s="2" t="s">
         <v>339</v>
@@ -13043,11 +13046,11 @@
       <c r="H150" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I150" s="0" t="s">
-        <v>9</v>
+      <c r="I150" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J150" s="0" t="s">
-        <v>9</v>
+        <v>531</v>
       </c>
       <c r="K150" s="2" t="s">
         <v>339</v>
@@ -13093,11 +13096,11 @@
       <c r="H151" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I151" s="0" t="s">
-        <v>9</v>
+      <c r="I151" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J151" s="0" t="s">
-        <v>9</v>
+        <v>533</v>
       </c>
       <c r="K151" s="2" t="s">
         <v>339</v>
@@ -13143,11 +13146,11 @@
       <c r="H152" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I152" s="0" t="s">
-        <v>9</v>
+      <c r="I152" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J152" s="0" t="s">
-        <v>9</v>
+        <v>535</v>
       </c>
       <c r="K152" s="2" t="s">
         <v>339</v>
@@ -13193,11 +13196,11 @@
       <c r="H153" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I153" s="0" t="s">
-        <v>9</v>
+      <c r="I153" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J153" s="0" t="s">
-        <v>9</v>
+        <v>537</v>
       </c>
       <c r="K153" s="2" t="s">
         <v>339</v>
@@ -13243,11 +13246,11 @@
       <c r="H154" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I154" s="0" t="s">
-        <v>9</v>
+      <c r="I154" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J154" s="0" t="s">
-        <v>9</v>
+        <v>539</v>
       </c>
       <c r="K154" s="2" t="s">
         <v>339</v>
@@ -13293,11 +13296,11 @@
       <c r="H155" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I155" s="0" t="s">
-        <v>9</v>
+      <c r="I155" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="J155" s="0" t="s">
-        <v>9</v>
+        <v>541</v>
       </c>
       <c r="K155" s="2" t="s">
         <v>339</v>
@@ -13343,11 +13346,11 @@
       <c r="H156" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I156" s="0" t="s">
-        <v>9</v>
+      <c r="I156" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="J156" s="0" t="s">
-        <v>9</v>
+        <v>543</v>
       </c>
       <c r="K156" s="2" t="s">
         <v>339</v>
@@ -13393,11 +13396,11 @@
       <c r="H157" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I157" s="0" t="s">
-        <v>9</v>
+      <c r="I157" s="1" t="s">
+        <v>281</v>
       </c>
       <c r="J157" s="0" t="s">
-        <v>9</v>
+        <v>544</v>
       </c>
       <c r="K157" s="2" t="s">
         <v>339</v>
@@ -13443,11 +13446,11 @@
       <c r="H158" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I158" s="0" t="s">
-        <v>9</v>
+      <c r="I158" s="1" t="s">
+        <v>283</v>
       </c>
       <c r="J158" s="0" t="s">
-        <v>9</v>
+        <v>545</v>
       </c>
       <c r="K158" s="2" t="s">
         <v>339</v>
@@ -13500,7 +13503,7 @@
         <v>9</v>
       </c>
       <c r="K159" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L159" s="0" t="s">
         <v>9</v>
@@ -13515,7 +13518,7 @@
         <v>337</v>
       </c>
       <c r="P159" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="160">
@@ -13550,7 +13553,7 @@
         <v>9</v>
       </c>
       <c r="K160" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L160" s="0" t="s">
         <v>9</v>
@@ -13565,7 +13568,7 @@
         <v>340</v>
       </c>
       <c r="P160" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="161">
@@ -13600,7 +13603,7 @@
         <v>9</v>
       </c>
       <c r="K161" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L161" s="0" t="s">
         <v>9</v>
@@ -13615,7 +13618,7 @@
         <v>340</v>
       </c>
       <c r="P161" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="162">
@@ -13650,7 +13653,7 @@
         <v>9</v>
       </c>
       <c r="K162" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L162" s="0" t="s">
         <v>9</v>
@@ -13665,7 +13668,7 @@
         <v>340</v>
       </c>
       <c r="P162" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="163">
@@ -13700,7 +13703,7 @@
         <v>9</v>
       </c>
       <c r="K163" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L163" s="0" t="s">
         <v>9</v>
@@ -13715,7 +13718,7 @@
         <v>340</v>
       </c>
       <c r="P163" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="164">
@@ -13750,7 +13753,7 @@
         <v>9</v>
       </c>
       <c r="K164" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L164" s="0" t="s">
         <v>9</v>
@@ -13765,7 +13768,7 @@
         <v>340</v>
       </c>
       <c r="P164" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="165">
@@ -13800,7 +13803,7 @@
         <v>9</v>
       </c>
       <c r="K165" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L165" s="0" t="s">
         <v>9</v>
@@ -13815,7 +13818,7 @@
         <v>340</v>
       </c>
       <c r="P165" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="166">
@@ -13850,7 +13853,7 @@
         <v>9</v>
       </c>
       <c r="K166" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L166" s="0" t="s">
         <v>9</v>
@@ -13865,7 +13868,7 @@
         <v>340</v>
       </c>
       <c r="P166" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="167">
@@ -13900,7 +13903,7 @@
         <v>9</v>
       </c>
       <c r="K167" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L167" s="0" t="s">
         <v>9</v>
@@ -13915,7 +13918,7 @@
         <v>340</v>
       </c>
       <c r="P167" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="168">
@@ -13950,7 +13953,7 @@
         <v>9</v>
       </c>
       <c r="K168" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L168" s="0" t="s">
         <v>9</v>
@@ -13965,7 +13968,7 @@
         <v>340</v>
       </c>
       <c r="P168" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="169">
@@ -14000,7 +14003,7 @@
         <v>9</v>
       </c>
       <c r="K169" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L169" s="0" t="s">
         <v>9</v>
@@ -14015,7 +14018,7 @@
         <v>340</v>
       </c>
       <c r="P169" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="170">
@@ -14050,7 +14053,7 @@
         <v>9</v>
       </c>
       <c r="K170" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L170" s="0" t="s">
         <v>9</v>
@@ -14065,7 +14068,7 @@
         <v>340</v>
       </c>
       <c r="P170" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="171">
@@ -14100,7 +14103,7 @@
         <v>9</v>
       </c>
       <c r="K171" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L171" s="0" t="s">
         <v>9</v>
@@ -14115,7 +14118,7 @@
         <v>340</v>
       </c>
       <c r="P171" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="172">
@@ -14150,7 +14153,7 @@
         <v>9</v>
       </c>
       <c r="K172" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L172" s="0" t="s">
         <v>9</v>
@@ -14165,7 +14168,7 @@
         <v>340</v>
       </c>
       <c r="P172" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="173">
@@ -14200,7 +14203,7 @@
         <v>9</v>
       </c>
       <c r="K173" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L173" s="0" t="s">
         <v>9</v>
@@ -14215,7 +14218,7 @@
         <v>340</v>
       </c>
       <c r="P173" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="174">
@@ -14250,7 +14253,7 @@
         <v>9</v>
       </c>
       <c r="K174" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L174" s="0" t="s">
         <v>9</v>
@@ -14265,7 +14268,7 @@
         <v>340</v>
       </c>
       <c r="P174" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="175">
@@ -14300,7 +14303,7 @@
         <v>9</v>
       </c>
       <c r="K175" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L175" s="0" t="s">
         <v>9</v>
@@ -14315,7 +14318,7 @@
         <v>340</v>
       </c>
       <c r="P175" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="176">
@@ -14350,7 +14353,7 @@
         <v>9</v>
       </c>
       <c r="K176" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L176" s="0" t="s">
         <v>9</v>
@@ -14365,7 +14368,7 @@
         <v>340</v>
       </c>
       <c r="P176" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="177">
@@ -14400,7 +14403,7 @@
         <v>9</v>
       </c>
       <c r="K177" s="2" t="s">
-        <v>339</v>
+        <v>546</v>
       </c>
       <c r="L177" s="0" t="s">
         <v>9</v>
@@ -14415,187 +14418,344 @@
         <v>337</v>
       </c>
       <c r="P177" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" display="ISSUE_TEMPLATE.md" r:id="rId2"/>
-    <hyperlink ref="A3" display="PULL_REQUEST_TEMPLATE.md" r:id="rId3"/>
-    <hyperlink ref="A4" display="index.md" r:id="rId4"/>
-    <hyperlink ref="A5" display="Microsoft.CSharp.RuntimeBinder.Binder.overwrite.md" r:id="rId5"/>
-    <hyperlink ref="A6" display="index.md" r:id="rId6"/>
-    <hyperlink ref="A7" display="products.md" r:id="rId7"/>
-    <hyperlink ref="A8" display="app-types.md" r:id="rId8"/>
-    <hyperlink ref="A9" display="creating-nuget-packages.md" r:id="rId9"/>
-    <hyperlink ref="A10" display="index.md" r:id="rId10"/>
-    <hyperlink ref="A11" display="reducing-dependencies.md" r:id="rId11"/>
-    <hyperlink ref="A12" display="getting-started.md" r:id="rId12"/>
-    <hyperlink ref="A13" display="index.md" r:id="rId13"/>
-    <hyperlink ref="A14" display="package-framework.png" r:id="rId14"/>
-    <hyperlink ref="A15" display="migrating-from-dnx.md" r:id="rId15"/>
-    <hyperlink ref="A16" display="packages.md" r:id="rId16"/>
-    <hyperlink ref="A17" display="index.md" r:id="rId17"/>
-    <hyperlink ref="A18" display="libraries.md" r:id="rId18"/>
-    <hyperlink ref="A19" display="project.pcl.png" r:id="rId19"/>
-    <hyperlink ref="A20" display="project.png" r:id="rId20"/>
-    <hyperlink ref="A21" display="project.xproj.different.png" r:id="rId21"/>
-    <hyperlink ref="A22" display="project.xproj.png" r:id="rId22"/>
-    <hyperlink ref="A23" display="project-structure.md" r:id="rId23"/>
-    <hyperlink ref="A24" display="third-party-deps.md" r:id="rId24"/>
-    <hyperlink ref="A25" display="rid-catalog.md" r:id="rId25"/>
-    <hyperlink ref="A26" display="sdk.md" r:id="rId26"/>
-    <hyperlink ref="A27" display="index.md" r:id="rId27"/>
-    <hyperlink ref="A28" display="unit-testing-with-dotnet-test.md" r:id="rId28"/>
-    <hyperlink ref="A29" display="dotnet-build.md" r:id="rId29"/>
-    <hyperlink ref="A30" display="dotnet-install-script.md" r:id="rId30"/>
-    <hyperlink ref="A31" display="dotnet-new.md" r:id="rId31"/>
-    <hyperlink ref="A32" display="dotnet-pack.md" r:id="rId32"/>
-    <hyperlink ref="A33" display="dotnet-publish.md" r:id="rId33"/>
-    <hyperlink ref="A34" display="dotnet-restore.md" r:id="rId34"/>
-    <hyperlink ref="A35" display="dotnet-run.md" r:id="rId35"/>
-    <hyperlink ref="A36" display="dotnet-test.md" r:id="rId36"/>
-    <hyperlink ref="A37" display="dotnet.md" r:id="rId37"/>
-    <hyperlink ref="A38" display="extensibility.md" r:id="rId38"/>
-    <hyperlink ref="A39" display="global-json.md" r:id="rId39"/>
-    <hyperlink ref="A40" display="index.md" r:id="rId40"/>
-    <hyperlink ref="A41" display="dotnet-test-discover.png" r:id="rId41"/>
-    <hyperlink ref="A42" display="dotnet-test-execute.png" r:id="rId42"/>
-    <hyperlink ref="A43" display="project-json.md" r:id="rId43"/>
-    <hyperlink ref="A44" display="telemetry.md" r:id="rId44"/>
-    <hyperlink ref="A45" display="test-protocol.md" r:id="rId45"/>
-    <hyperlink ref="A46" display="using-ci-with-cli.md" r:id="rId46"/>
-    <hyperlink ref="A47" display="aspnet-core.md" r:id="rId47"/>
-    <hyperlink ref="A48" display="index.md" r:id="rId48"/>
-    <hyperlink ref="A49" display="libraries.md" r:id="rId49"/>
-    <hyperlink ref="A50" display="managing-package-dependency-versions.md" r:id="rId50"/>
-    <hyperlink ref="A51" display="new-project-dialog-class-library-portable.png" r:id="rId51"/>
-    <hyperlink ref="A52" display="pcl-targets-dialog-net46-aspnetcore10.png" r:id="rId52"/>
-    <hyperlink ref="A53" display="vscodedebugger.png" r:id="rId53"/>
-    <hyperlink ref="A54" display="target-dotnetcore-with-msbuild.md" r:id="rId54"/>
-    <hyperlink ref="A55" display="using-on-macos.md" r:id="rId55"/>
-    <hyperlink ref="A56" display="using-on-windows.md" r:id="rId56"/>
-    <hyperlink ref="A57" display="using-with-xplat-cli.md" r:id="rId57"/>
-    <hyperlink ref="A58" display="index.md" r:id="rId58"/>
-    <hyperlink ref="A59" display="windows-prerequisites.md" r:id="rId59"/>
-    <hyperlink ref="A60" display="async.md" r:id="rId60"/>
-    <hyperlink ref="A61" display="csharp-6.md" r:id="rId61"/>
-    <hyperlink ref="A62" display="delegate-class.md" r:id="rId62"/>
-    <hyperlink ref="A63" display="delegates-events.md" r:id="rId63"/>
-    <hyperlink ref="A64" display="delegates-overview.md" r:id="rId64"/>
-    <hyperlink ref="A65" display="delegates-patterns.md" r:id="rId65"/>
-    <hyperlink ref="A66" display="delegates-strongly-typed.md" r:id="rId66"/>
-    <hyperlink ref="A67" display="distinguish-delegates-events.md" r:id="rId67"/>
-    <hyperlink ref="A68" display="event-pattern.md" r:id="rId68"/>
-    <hyperlink ref="A69" display="events-overview.md" r:id="rId69"/>
-    <hyperlink ref="A70" display="expression-classes.md" r:id="rId70"/>
-    <hyperlink ref="A71" display="expression-trees-building.md" r:id="rId71"/>
-    <hyperlink ref="A72" display="expression-trees-execution.md" r:id="rId72"/>
-    <hyperlink ref="A73" display="expression-trees-explained.md" r:id="rId73"/>
-    <hyperlink ref="A74" display="expression-trees-interpreting.md" r:id="rId74"/>
-    <hyperlink ref="A75" display="expression-trees-summary.md" r:id="rId75"/>
-    <hyperlink ref="A76" display="expression-trees-translating.md" r:id="rId76"/>
-    <hyperlink ref="A77" display="expression-trees.md" r:id="rId77"/>
-    <hyperlink ref="A78" display="implicitly-typed-lambda-expressions.md" r:id="rId78"/>
-    <hyperlink ref="A79" display="indexers.md" r:id="rId79"/>
-    <hyperlink ref="A80" display="iterators.md" r:id="rId80"/>
-    <hyperlink ref="A81" display="modern-events.md" r:id="rId81"/>
-    <hyperlink ref="A82" display="properties.md" r:id="rId82"/>
-    <hyperlink ref="A83" display="console-teleprompter.md" r:id="rId83"/>
-    <hyperlink ref="A84" display="console-webapiclient.md" r:id="rId84"/>
-    <hyperlink ref="A85" display="index.md" r:id="rId85"/>
-    <hyperlink ref="A86" display="microservices.md" r:id="rId86"/>
-    <hyperlink ref="A87" display="working-with-linq.md" r:id="rId87"/>
-    <hyperlink ref="A88" display="async.md" r:id="rId88"/>
-    <hyperlink ref="A89" display="getting-started-netcore.md" r:id="rId89"/>
-    <hyperlink ref="A90" display="index.md" r:id="rId90"/>
-    <hyperlink ref="A91" display="corefx-platforms-loc.png" r:id="rId91"/>
-    <hyperlink ref="A92" display="index.md" r:id="rId92"/>
-    <hyperlink ref="A93" display="assembly-format.md" r:id="rId93"/>
-    <hyperlink ref="A94" display="async-in-depth.md" r:id="rId94"/>
-    <hyperlink ref="A95" display="async.md" r:id="rId95"/>
-    <hyperlink ref="A96" display="class-libraries.md" r:id="rId96"/>
-    <hyperlink ref="A97" display="clr.md" r:id="rId97"/>
-    <hyperlink ref="A98" display="commonly-used-collection-types.md" r:id="rId98"/>
-    <hyperlink ref="A99" display="comparisons-and-sorts-within-collections.md" r:id="rId99"/>
-    <hyperlink ref="A100" display="hashtable-and-dictionary-collection-types.md" r:id="rId100"/>
-    <hyperlink ref="A101" display="index.md" r:id="rId101"/>
-    <hyperlink ref="A102" display="selecting-a-collection-class.md" r:id="rId102"/>
-    <hyperlink ref="A103" display="sorted-collection-types.md" r:id="rId103"/>
-    <hyperlink ref="A104" display="blockingcollection-overview.md" r:id="rId104"/>
-    <hyperlink ref="A105" display="how-to-add-and-remove-items.md" r:id="rId105"/>
-    <hyperlink ref="A106" display="how-to-add-and-take-items.md" r:id="rId106"/>
-    <hyperlink ref="A107" display="how-to-add-bounding-and-blocking.md" r:id="rId107"/>
-    <hyperlink ref="A108" display="how-to-create-an-object-pool.md" r:id="rId108"/>
-    <hyperlink ref="A109" display="how-to-use-arrays-of-blockingcollections.md" r:id="rId109"/>
-    <hyperlink ref="A110" display="how-to-use-foreach-to-remove.md" r:id="rId110"/>
-    <hyperlink ref="A111" display="index.md" r:id="rId111"/>
-    <hyperlink ref="A112" display="when-to-use-a-thread-safe-collection.md" r:id="rId112"/>
-    <hyperlink ref="A113" display="when-to-use-generic-collections.md" r:id="rId113"/>
-    <hyperlink ref="A114" display="common-type-system.md" r:id="rId114"/>
-    <hyperlink ref="A115" display="delegates-lambdas.md" r:id="rId115"/>
-    <hyperlink ref="A116" display="exceptions.md" r:id="rId116"/>
-    <hyperlink ref="A117" display="framework-libraries.md" r:id="rId117"/>
-    <hyperlink ref="A118" display="frameworks.md" r:id="rId118"/>
-    <hyperlink ref="A119" display="gc-overview.md" r:id="rId119"/>
-    <hyperlink ref="A120" display="generics.md" r:id="rId120"/>
-    <hyperlink ref="A121" display="index.md" r:id="rId121"/>
-    <hyperlink ref="A122" display="library.md" r:id="rId122"/>
-    <hyperlink ref="A123" display="managed-code.md" r:id="rId123"/>
-    <hyperlink ref="A124" display="assembly-headers.png" r:id="rId124"/>
-    <hyperlink ref="A125" display="portability-report.png" r:id="rId125"/>
-    <hyperlink ref="A126" display="portability-screenshot.png" r:id="rId126"/>
-    <hyperlink ref="A127" display="portability-solution-explorer.png" r:id="rId127"/>
-    <hyperlink ref="A128" display="plinq-diagram.png" r:id="rId128"/>
-    <hyperlink ref="A129" display="native-interop.md" r:id="rId129"/>
-    <hyperlink ref="A130" display="numerics.md" r:id="rId130"/>
-    <hyperlink ref="A131" display="portability-analyzer.md" r:id="rId131"/>
-    <hyperlink ref="A132" display="using-linq.md" r:id="rId132"/>
-    <hyperlink ref="A133" display="welcome.md" r:id="rId133"/>
-    <hyperlink ref="A134" display="index.md" r:id="rId134"/>
-    <hyperlink ref="A135" display="README.md" r:id="rId135"/>
-    <hyperlink ref="A136" display="README.md" r:id="rId136"/>
-    <hyperlink ref="A137" display="README.md" r:id="rId137"/>
-    <hyperlink ref="A138" display="README.md" r:id="rId138"/>
-    <hyperlink ref="A139" display="README.md" r:id="rId139"/>
-    <hyperlink ref="A140" display="README.md" r:id="rId140"/>
-    <hyperlink ref="A141" display="README.md" r:id="rId141"/>
-    <hyperlink ref="A142" display="README.md" r:id="rId142"/>
-    <hyperlink ref="A143" display="README.md" r:id="rId143"/>
-    <hyperlink ref="A144" display="README.md" r:id="rId144"/>
-    <hyperlink ref="A145" display="README.md" r:id="rId145"/>
-    <hyperlink ref="A146" display="README.md" r:id="rId146"/>
-    <hyperlink ref="A147" display="README.md" r:id="rId147"/>
-    <hyperlink ref="A148" display="README.md" r:id="rId148"/>
-    <hyperlink ref="A149" display="README.md" r:id="rId149"/>
-    <hyperlink ref="A150" display="README.md" r:id="rId150"/>
-    <hyperlink ref="A151" display="README.md" r:id="rId151"/>
-    <hyperlink ref="A152" display="README.md" r:id="rId152"/>
-    <hyperlink ref="A153" display="README.md" r:id="rId153"/>
-    <hyperlink ref="A154" display="README.md" r:id="rId154"/>
-    <hyperlink ref="A155" display="README.md" r:id="rId155"/>
-    <hyperlink ref="A156" display="template.md" r:id="rId156"/>
-    <hyperlink ref="A157" display="voice-tone.md" r:id="rId157"/>
-    <hyperlink ref="A158" display="TOC.md" r:id="rId158"/>
-    <hyperlink ref="A159" display="CONTRIBUTING.md" r:id="rId159"/>
-    <hyperlink ref="A160" display="applications.md" r:id="rId160"/>
-    <hyperlink ref="A161" display="nuget-packages.md" r:id="rId161"/>
-    <hyperlink ref="A162" display="cli-console-app-tutorial-advanced.md" r:id="rId162"/>
-    <hyperlink ref="A163" display="libraries-with-vs.md" r:id="rId163"/>
-    <hyperlink ref="A164" display="servicing.md" r:id="rId164"/>
-    <hyperlink ref="A165" display="codedoc.md" r:id="rId165"/>
-    <hyperlink ref="A166" display="concepts.md" r:id="rId166"/>
-    <hyperlink ref="A167" display="features.md" r:id="rId167"/>
-    <hyperlink ref="A168" display="generics.md" r:id="rId168"/>
-    <hyperlink ref="A169" display="index.md" r:id="rId169"/>
-    <hyperlink ref="A170" display="interop.md" r:id="rId170"/>
-    <hyperlink ref="A171" display="lambda-expressions.md" r:id="rId171"/>
-    <hyperlink ref="A172" display="linq.md" r:id="rId172"/>
-    <hyperlink ref="A173" display="parallel.md" r:id="rId173"/>
-    <hyperlink ref="A174" display="reflection.md" r:id="rId174"/>
-    <hyperlink ref="A175" display="syntax.md" r:id="rId175"/>
-    <hyperlink ref="A176" display="type-system.md" r:id="rId176"/>
-    <hyperlink ref="A177" display="toc.md" r:id="rId177"/>
+    <hyperlink ref="I2" display="ISSUE_TEMPLATE.md" r:id="rId3"/>
+    <hyperlink ref="A3" display="PULL_REQUEST_TEMPLATE.md" r:id="rId4"/>
+    <hyperlink ref="I3" display="PULL_REQUEST_TEMPLATE.md" r:id="rId5"/>
+    <hyperlink ref="A4" display="index.md" r:id="rId6"/>
+    <hyperlink ref="I4" display="index.md" r:id="rId7"/>
+    <hyperlink ref="A5" display="Microsoft.CSharp.RuntimeBinder.Binder.overwrite.md" r:id="rId8"/>
+    <hyperlink ref="I5" display="Microsoft.CSharp.RuntimeBinder.Binder.overwrite.md" r:id="rId9"/>
+    <hyperlink ref="A6" display="index.md" r:id="rId10"/>
+    <hyperlink ref="I6" display="index.md" r:id="rId11"/>
+    <hyperlink ref="A7" display="products.md" r:id="rId12"/>
+    <hyperlink ref="I7" display="products.md" r:id="rId13"/>
+    <hyperlink ref="A8" display="app-types.md" r:id="rId14"/>
+    <hyperlink ref="I8" display="app-types.md" r:id="rId15"/>
+    <hyperlink ref="A9" display="creating-nuget-packages.md" r:id="rId16"/>
+    <hyperlink ref="I9" display="creating-nuget-packages.md" r:id="rId17"/>
+    <hyperlink ref="A10" display="index.md" r:id="rId18"/>
+    <hyperlink ref="I10" display="index.md" r:id="rId19"/>
+    <hyperlink ref="A11" display="reducing-dependencies.md" r:id="rId20"/>
+    <hyperlink ref="I11" display="reducing-dependencies.md" r:id="rId21"/>
+    <hyperlink ref="A12" display="getting-started.md" r:id="rId22"/>
+    <hyperlink ref="I12" display="getting-started.md" r:id="rId23"/>
+    <hyperlink ref="A13" display="index.md" r:id="rId24"/>
+    <hyperlink ref="I13" display="index.md" r:id="rId25"/>
+    <hyperlink ref="A14" display="package-framework.png" r:id="rId26"/>
+    <hyperlink ref="I14" display="package-framework.png" r:id="rId27"/>
+    <hyperlink ref="A15" display="migrating-from-dnx.md" r:id="rId28"/>
+    <hyperlink ref="I15" display="migrating-from-dnx.md" r:id="rId29"/>
+    <hyperlink ref="A16" display="packages.md" r:id="rId30"/>
+    <hyperlink ref="I16" display="packages.md" r:id="rId31"/>
+    <hyperlink ref="A17" display="index.md" r:id="rId32"/>
+    <hyperlink ref="I17" display="index.md" r:id="rId33"/>
+    <hyperlink ref="A18" display="libraries.md" r:id="rId34"/>
+    <hyperlink ref="I18" display="libraries.md" r:id="rId35"/>
+    <hyperlink ref="A19" display="project.pcl.png" r:id="rId36"/>
+    <hyperlink ref="I19" display="project.pcl.png" r:id="rId37"/>
+    <hyperlink ref="A20" display="project.png" r:id="rId38"/>
+    <hyperlink ref="I20" display="project.png" r:id="rId39"/>
+    <hyperlink ref="A21" display="project.xproj.different.png" r:id="rId40"/>
+    <hyperlink ref="I21" display="project.xproj.different.png" r:id="rId41"/>
+    <hyperlink ref="A22" display="project.xproj.png" r:id="rId42"/>
+    <hyperlink ref="I22" display="project.xproj.png" r:id="rId43"/>
+    <hyperlink ref="A23" display="project-structure.md" r:id="rId44"/>
+    <hyperlink ref="I23" display="project-structure.md" r:id="rId45"/>
+    <hyperlink ref="A24" display="third-party-deps.md" r:id="rId46"/>
+    <hyperlink ref="I24" display="third-party-deps.md" r:id="rId47"/>
+    <hyperlink ref="A25" display="rid-catalog.md" r:id="rId48"/>
+    <hyperlink ref="I25" display="rid-catalog.md" r:id="rId49"/>
+    <hyperlink ref="A26" display="sdk.md" r:id="rId50"/>
+    <hyperlink ref="I26" display="sdk.md" r:id="rId51"/>
+    <hyperlink ref="A27" display="index.md" r:id="rId52"/>
+    <hyperlink ref="I27" display="index.md" r:id="rId53"/>
+    <hyperlink ref="A28" display="unit-testing-with-dotnet-test.md" r:id="rId54"/>
+    <hyperlink ref="I28" display="unit-testing-with-dotnet-test.md" r:id="rId55"/>
+    <hyperlink ref="A29" display="dotnet-build.md" r:id="rId56"/>
+    <hyperlink ref="I29" display="dotnet-build.md" r:id="rId57"/>
+    <hyperlink ref="A30" display="dotnet-install-script.md" r:id="rId58"/>
+    <hyperlink ref="I30" display="dotnet-install-script.md" r:id="rId59"/>
+    <hyperlink ref="A31" display="dotnet-new.md" r:id="rId60"/>
+    <hyperlink ref="I31" display="dotnet-new.md" r:id="rId61"/>
+    <hyperlink ref="A32" display="dotnet-pack.md" r:id="rId62"/>
+    <hyperlink ref="I32" display="dotnet-pack.md" r:id="rId63"/>
+    <hyperlink ref="A33" display="dotnet-publish.md" r:id="rId64"/>
+    <hyperlink ref="I33" display="dotnet-publish.md" r:id="rId65"/>
+    <hyperlink ref="A34" display="dotnet-restore.md" r:id="rId66"/>
+    <hyperlink ref="I34" display="dotnet-restore.md" r:id="rId67"/>
+    <hyperlink ref="A35" display="dotnet-run.md" r:id="rId68"/>
+    <hyperlink ref="I35" display="dotnet-run.md" r:id="rId69"/>
+    <hyperlink ref="A36" display="dotnet-test.md" r:id="rId70"/>
+    <hyperlink ref="I36" display="dotnet-test.md" r:id="rId71"/>
+    <hyperlink ref="A37" display="dotnet.md" r:id="rId72"/>
+    <hyperlink ref="I37" display="dotnet.md" r:id="rId73"/>
+    <hyperlink ref="A38" display="extensibility.md" r:id="rId74"/>
+    <hyperlink ref="I38" display="extensibility.md" r:id="rId75"/>
+    <hyperlink ref="A39" display="global-json.md" r:id="rId76"/>
+    <hyperlink ref="I39" display="global-json.md" r:id="rId77"/>
+    <hyperlink ref="A40" display="index.md" r:id="rId78"/>
+    <hyperlink ref="I40" display="index.md" r:id="rId79"/>
+    <hyperlink ref="A41" display="dotnet-test-discover.png" r:id="rId80"/>
+    <hyperlink ref="I41" display="dotnet-test-discover.png" r:id="rId81"/>
+    <hyperlink ref="A42" display="dotnet-test-execute.png" r:id="rId82"/>
+    <hyperlink ref="I42" display="dotnet-test-execute.png" r:id="rId83"/>
+    <hyperlink ref="A43" display="project-json.md" r:id="rId84"/>
+    <hyperlink ref="I43" display="project-json.md" r:id="rId85"/>
+    <hyperlink ref="A44" display="telemetry.md" r:id="rId86"/>
+    <hyperlink ref="I44" display="telemetry.md" r:id="rId87"/>
+    <hyperlink ref="A45" display="test-protocol.md" r:id="rId88"/>
+    <hyperlink ref="I45" display="test-protocol.md" r:id="rId89"/>
+    <hyperlink ref="A46" display="using-ci-with-cli.md" r:id="rId90"/>
+    <hyperlink ref="I46" display="using-ci-with-cli.md" r:id="rId91"/>
+    <hyperlink ref="A47" display="aspnet-core.md" r:id="rId92"/>
+    <hyperlink ref="I47" display="aspnet-core.md" r:id="rId93"/>
+    <hyperlink ref="A48" display="index.md" r:id="rId94"/>
+    <hyperlink ref="I48" display="index.md" r:id="rId95"/>
+    <hyperlink ref="A49" display="libraries.md" r:id="rId96"/>
+    <hyperlink ref="I49" display="libraries.md" r:id="rId97"/>
+    <hyperlink ref="A50" display="managing-package-dependency-versions.md" r:id="rId98"/>
+    <hyperlink ref="I50" display="managing-package-dependency-versions.md" r:id="rId99"/>
+    <hyperlink ref="A51" display="new-project-dialog-class-library-portable.png" r:id="rId100"/>
+    <hyperlink ref="I51" display="new-project-dialog-class-library-portable.png" r:id="rId101"/>
+    <hyperlink ref="A52" display="pcl-targets-dialog-net46-aspnetcore10.png" r:id="rId102"/>
+    <hyperlink ref="I52" display="pcl-targets-dialog-net46-aspnetcore10.png" r:id="rId103"/>
+    <hyperlink ref="A53" display="vscodedebugger.png" r:id="rId104"/>
+    <hyperlink ref="I53" display="vscodedebugger.png" r:id="rId105"/>
+    <hyperlink ref="A54" display="target-dotnetcore-with-msbuild.md" r:id="rId106"/>
+    <hyperlink ref="I54" display="target-dotnetcore-with-msbuild.md" r:id="rId107"/>
+    <hyperlink ref="A55" display="using-on-macos.md" r:id="rId108"/>
+    <hyperlink ref="I55" display="using-on-macos.md" r:id="rId109"/>
+    <hyperlink ref="A56" display="using-on-windows.md" r:id="rId110"/>
+    <hyperlink ref="I56" display="using-on-windows.md" r:id="rId111"/>
+    <hyperlink ref="A57" display="using-with-xplat-cli.md" r:id="rId112"/>
+    <hyperlink ref="I57" display="using-with-xplat-cli.md" r:id="rId113"/>
+    <hyperlink ref="A58" display="index.md" r:id="rId114"/>
+    <hyperlink ref="I58" display="index.md" r:id="rId115"/>
+    <hyperlink ref="A59" display="windows-prerequisites.md" r:id="rId116"/>
+    <hyperlink ref="I59" display="windows-prerequisites.md" r:id="rId117"/>
+    <hyperlink ref="A60" display="async.md" r:id="rId118"/>
+    <hyperlink ref="I60" display="async.md" r:id="rId119"/>
+    <hyperlink ref="A61" display="csharp-6.md" r:id="rId120"/>
+    <hyperlink ref="I61" display="csharp-6.md" r:id="rId121"/>
+    <hyperlink ref="A62" display="delegate-class.md" r:id="rId122"/>
+    <hyperlink ref="I62" display="delegate-class.md" r:id="rId123"/>
+    <hyperlink ref="A63" display="delegates-events.md" r:id="rId124"/>
+    <hyperlink ref="I63" display="delegates-events.md" r:id="rId125"/>
+    <hyperlink ref="A64" display="delegates-overview.md" r:id="rId126"/>
+    <hyperlink ref="I64" display="delegates-overview.md" r:id="rId127"/>
+    <hyperlink ref="A65" display="delegates-patterns.md" r:id="rId128"/>
+    <hyperlink ref="I65" display="delegates-patterns.md" r:id="rId129"/>
+    <hyperlink ref="A66" display="delegates-strongly-typed.md" r:id="rId130"/>
+    <hyperlink ref="I66" display="delegates-strongly-typed.md" r:id="rId131"/>
+    <hyperlink ref="A67" display="distinguish-delegates-events.md" r:id="rId132"/>
+    <hyperlink ref="I67" display="distinguish-delegates-events.md" r:id="rId133"/>
+    <hyperlink ref="A68" display="event-pattern.md" r:id="rId134"/>
+    <hyperlink ref="I68" display="event-pattern.md" r:id="rId135"/>
+    <hyperlink ref="A69" display="events-overview.md" r:id="rId136"/>
+    <hyperlink ref="I69" display="events-overview.md" r:id="rId137"/>
+    <hyperlink ref="A70" display="expression-classes.md" r:id="rId138"/>
+    <hyperlink ref="I70" display="expression-classes.md" r:id="rId139"/>
+    <hyperlink ref="A71" display="expression-trees-building.md" r:id="rId140"/>
+    <hyperlink ref="I71" display="expression-trees-building.md" r:id="rId141"/>
+    <hyperlink ref="A72" display="expression-trees-execution.md" r:id="rId142"/>
+    <hyperlink ref="I72" display="expression-trees-execution.md" r:id="rId143"/>
+    <hyperlink ref="A73" display="expression-trees-explained.md" r:id="rId144"/>
+    <hyperlink ref="I73" display="expression-trees-explained.md" r:id="rId145"/>
+    <hyperlink ref="A74" display="expression-trees-interpreting.md" r:id="rId146"/>
+    <hyperlink ref="I74" display="expression-trees-interpreting.md" r:id="rId147"/>
+    <hyperlink ref="A75" display="expression-trees-summary.md" r:id="rId148"/>
+    <hyperlink ref="I75" display="expression-trees-summary.md" r:id="rId149"/>
+    <hyperlink ref="A76" display="expression-trees-translating.md" r:id="rId150"/>
+    <hyperlink ref="I76" display="expression-trees-translating.md" r:id="rId151"/>
+    <hyperlink ref="A77" display="expression-trees.md" r:id="rId152"/>
+    <hyperlink ref="I77" display="expression-trees.md" r:id="rId153"/>
+    <hyperlink ref="A78" display="implicitly-typed-lambda-expressions.md" r:id="rId154"/>
+    <hyperlink ref="I78" display="implicitly-typed-lambda-expressions.md" r:id="rId155"/>
+    <hyperlink ref="A79" display="indexers.md" r:id="rId156"/>
+    <hyperlink ref="I79" display="indexers.md" r:id="rId157"/>
+    <hyperlink ref="A80" display="iterators.md" r:id="rId158"/>
+    <hyperlink ref="I80" display="iterators.md" r:id="rId159"/>
+    <hyperlink ref="A81" display="modern-events.md" r:id="rId160"/>
+    <hyperlink ref="I81" display="modern-events.md" r:id="rId161"/>
+    <hyperlink ref="A82" display="properties.md" r:id="rId162"/>
+    <hyperlink ref="I82" display="properties.md" r:id="rId163"/>
+    <hyperlink ref="A83" display="console-teleprompter.md" r:id="rId164"/>
+    <hyperlink ref="I83" display="console-teleprompter.md" r:id="rId165"/>
+    <hyperlink ref="A84" display="console-webapiclient.md" r:id="rId166"/>
+    <hyperlink ref="I84" display="console-webapiclient.md" r:id="rId167"/>
+    <hyperlink ref="A85" display="index.md" r:id="rId168"/>
+    <hyperlink ref="I85" display="index.md" r:id="rId169"/>
+    <hyperlink ref="A86" display="microservices.md" r:id="rId170"/>
+    <hyperlink ref="I86" display="microservices.md" r:id="rId171"/>
+    <hyperlink ref="A87" display="working-with-linq.md" r:id="rId172"/>
+    <hyperlink ref="I87" display="working-with-linq.md" r:id="rId173"/>
+    <hyperlink ref="A88" display="async.md" r:id="rId174"/>
+    <hyperlink ref="I88" display="async.md" r:id="rId175"/>
+    <hyperlink ref="A89" display="getting-started-netcore.md" r:id="rId176"/>
+    <hyperlink ref="I89" display="getting-started-netcore.md" r:id="rId177"/>
+    <hyperlink ref="A90" display="index.md" r:id="rId178"/>
+    <hyperlink ref="I90" display="index.md" r:id="rId179"/>
+    <hyperlink ref="A91" display="corefx-platforms-loc.png" r:id="rId180"/>
+    <hyperlink ref="I91" display="corefx-platforms-loc.png" r:id="rId181"/>
+    <hyperlink ref="A92" display="index.md" r:id="rId182"/>
+    <hyperlink ref="I92" display="index.md" r:id="rId183"/>
+    <hyperlink ref="A93" display="assembly-format.md" r:id="rId184"/>
+    <hyperlink ref="I93" display="assembly-format.md" r:id="rId185"/>
+    <hyperlink ref="A94" display="async-in-depth.md" r:id="rId186"/>
+    <hyperlink ref="I94" display="async-in-depth.md" r:id="rId187"/>
+    <hyperlink ref="A95" display="async.md" r:id="rId188"/>
+    <hyperlink ref="I95" display="async.md" r:id="rId189"/>
+    <hyperlink ref="A96" display="class-libraries.md" r:id="rId190"/>
+    <hyperlink ref="I96" display="class-libraries.md" r:id="rId191"/>
+    <hyperlink ref="A97" display="clr.md" r:id="rId192"/>
+    <hyperlink ref="I97" display="clr.md" r:id="rId193"/>
+    <hyperlink ref="A98" display="commonly-used-collection-types.md" r:id="rId194"/>
+    <hyperlink ref="I98" display="commonly-used-collection-types.md" r:id="rId195"/>
+    <hyperlink ref="A99" display="comparisons-and-sorts-within-collections.md" r:id="rId196"/>
+    <hyperlink ref="I99" display="comparisons-and-sorts-within-collections.md" r:id="rId197"/>
+    <hyperlink ref="A100" display="hashtable-and-dictionary-collection-types.md" r:id="rId198"/>
+    <hyperlink ref="I100" display="hashtable-and-dictionary-collection-types.md" r:id="rId199"/>
+    <hyperlink ref="A101" display="index.md" r:id="rId200"/>
+    <hyperlink ref="I101" display="index.md" r:id="rId201"/>
+    <hyperlink ref="A102" display="selecting-a-collection-class.md" r:id="rId202"/>
+    <hyperlink ref="I102" display="selecting-a-collection-class.md" r:id="rId203"/>
+    <hyperlink ref="A103" display="sorted-collection-types.md" r:id="rId204"/>
+    <hyperlink ref="I103" display="sorted-collection-types.md" r:id="rId205"/>
+    <hyperlink ref="A104" display="blockingcollection-overview.md" r:id="rId206"/>
+    <hyperlink ref="I104" display="blockingcollection-overview.md" r:id="rId207"/>
+    <hyperlink ref="A105" display="how-to-add-and-remove-items.md" r:id="rId208"/>
+    <hyperlink ref="I105" display="how-to-add-and-remove-items.md" r:id="rId209"/>
+    <hyperlink ref="A106" display="how-to-add-and-take-items.md" r:id="rId210"/>
+    <hyperlink ref="I106" display="how-to-add-and-take-items.md" r:id="rId211"/>
+    <hyperlink ref="A107" display="how-to-add-bounding-and-blocking.md" r:id="rId212"/>
+    <hyperlink ref="I107" display="how-to-add-bounding-and-blocking.md" r:id="rId213"/>
+    <hyperlink ref="A108" display="how-to-create-an-object-pool.md" r:id="rId214"/>
+    <hyperlink ref="I108" display="how-to-create-an-object-pool.md" r:id="rId215"/>
+    <hyperlink ref="A109" display="how-to-use-arrays-of-blockingcollections.md" r:id="rId216"/>
+    <hyperlink ref="I109" display="how-to-use-arrays-of-blockingcollections.md" r:id="rId217"/>
+    <hyperlink ref="A110" display="how-to-use-foreach-to-remove.md" r:id="rId218"/>
+    <hyperlink ref="I110" display="how-to-use-foreach-to-remove.md" r:id="rId219"/>
+    <hyperlink ref="A111" display="index.md" r:id="rId220"/>
+    <hyperlink ref="I111" display="index.md" r:id="rId221"/>
+    <hyperlink ref="A112" display="when-to-use-a-thread-safe-collection.md" r:id="rId222"/>
+    <hyperlink ref="I112" display="when-to-use-a-thread-safe-collection.md" r:id="rId223"/>
+    <hyperlink ref="A113" display="when-to-use-generic-collections.md" r:id="rId224"/>
+    <hyperlink ref="I113" display="when-to-use-generic-collections.md" r:id="rId225"/>
+    <hyperlink ref="A114" display="common-type-system.md" r:id="rId226"/>
+    <hyperlink ref="I114" display="common-type-system.md" r:id="rId227"/>
+    <hyperlink ref="A115" display="delegates-lambdas.md" r:id="rId228"/>
+    <hyperlink ref="I115" display="delegates-lambdas.md" r:id="rId229"/>
+    <hyperlink ref="A116" display="exceptions.md" r:id="rId230"/>
+    <hyperlink ref="I116" display="exceptions.md" r:id="rId231"/>
+    <hyperlink ref="A117" display="framework-libraries.md" r:id="rId232"/>
+    <hyperlink ref="I117" display="framework-libraries.md" r:id="rId233"/>
+    <hyperlink ref="A118" display="frameworks.md" r:id="rId234"/>
+    <hyperlink ref="I118" display="frameworks.md" r:id="rId235"/>
+    <hyperlink ref="A119" display="gc-overview.md" r:id="rId236"/>
+    <hyperlink ref="I119" display="gc-overview.md" r:id="rId237"/>
+    <hyperlink ref="A120" display="generics.md" r:id="rId238"/>
+    <hyperlink ref="I120" display="generics.md" r:id="rId239"/>
+    <hyperlink ref="A121" display="index.md" r:id="rId240"/>
+    <hyperlink ref="I121" display="index.md" r:id="rId241"/>
+    <hyperlink ref="A122" display="library.md" r:id="rId242"/>
+    <hyperlink ref="I122" display="library.md" r:id="rId243"/>
+    <hyperlink ref="A123" display="managed-code.md" r:id="rId244"/>
+    <hyperlink ref="I123" display="managed-code.md" r:id="rId245"/>
+    <hyperlink ref="A124" display="assembly-headers.png" r:id="rId246"/>
+    <hyperlink ref="I124" display="assembly-headers.png" r:id="rId247"/>
+    <hyperlink ref="A125" display="portability-report.png" r:id="rId248"/>
+    <hyperlink ref="I125" display="portability-report.png" r:id="rId249"/>
+    <hyperlink ref="A126" display="portability-screenshot.png" r:id="rId250"/>
+    <hyperlink ref="I126" display="portability-screenshot.png" r:id="rId251"/>
+    <hyperlink ref="A127" display="portability-solution-explorer.png" r:id="rId252"/>
+    <hyperlink ref="I127" display="portability-solution-explorer.png" r:id="rId253"/>
+    <hyperlink ref="A128" display="plinq-diagram.png" r:id="rId254"/>
+    <hyperlink ref="I128" display="plinq-diagram.png" r:id="rId255"/>
+    <hyperlink ref="A129" display="native-interop.md" r:id="rId256"/>
+    <hyperlink ref="I129" display="native-interop.md" r:id="rId257"/>
+    <hyperlink ref="A130" display="numerics.md" r:id="rId258"/>
+    <hyperlink ref="I130" display="numerics.md" r:id="rId259"/>
+    <hyperlink ref="A131" display="portability-analyzer.md" r:id="rId260"/>
+    <hyperlink ref="I131" display="portability-analyzer.md" r:id="rId261"/>
+    <hyperlink ref="A132" display="using-linq.md" r:id="rId262"/>
+    <hyperlink ref="I132" display="using-linq.md" r:id="rId263"/>
+    <hyperlink ref="A133" display="welcome.md" r:id="rId264"/>
+    <hyperlink ref="I133" display="welcome.md" r:id="rId265"/>
+    <hyperlink ref="A134" display="index.md" r:id="rId266"/>
+    <hyperlink ref="I134" display="index.md" r:id="rId267"/>
+    <hyperlink ref="A135" display="README.md" r:id="rId268"/>
+    <hyperlink ref="I135" display="README.md" r:id="rId269"/>
+    <hyperlink ref="A136" display="README.md" r:id="rId270"/>
+    <hyperlink ref="I136" display="README.md" r:id="rId271"/>
+    <hyperlink ref="A137" display="README.md" r:id="rId272"/>
+    <hyperlink ref="I137" display="README.md" r:id="rId273"/>
+    <hyperlink ref="A138" display="README.md" r:id="rId274"/>
+    <hyperlink ref="I138" display="README.md" r:id="rId275"/>
+    <hyperlink ref="A139" display="README.md" r:id="rId276"/>
+    <hyperlink ref="I139" display="README.md" r:id="rId277"/>
+    <hyperlink ref="A140" display="README.md" r:id="rId278"/>
+    <hyperlink ref="I140" display="README.md" r:id="rId279"/>
+    <hyperlink ref="A141" display="README.md" r:id="rId280"/>
+    <hyperlink ref="I141" display="README.md" r:id="rId281"/>
+    <hyperlink ref="A142" display="README.md" r:id="rId282"/>
+    <hyperlink ref="I142" display="README.md" r:id="rId283"/>
+    <hyperlink ref="A143" display="README.md" r:id="rId284"/>
+    <hyperlink ref="I143" display="README.md" r:id="rId285"/>
+    <hyperlink ref="A144" display="README.md" r:id="rId286"/>
+    <hyperlink ref="I144" display="README.md" r:id="rId287"/>
+    <hyperlink ref="A145" display="README.md" r:id="rId288"/>
+    <hyperlink ref="I145" display="README.md" r:id="rId289"/>
+    <hyperlink ref="A146" display="README.md" r:id="rId290"/>
+    <hyperlink ref="I146" display="README.md" r:id="rId291"/>
+    <hyperlink ref="A147" display="README.md" r:id="rId292"/>
+    <hyperlink ref="I147" display="README.md" r:id="rId293"/>
+    <hyperlink ref="A148" display="README.md" r:id="rId294"/>
+    <hyperlink ref="I148" display="README.md" r:id="rId295"/>
+    <hyperlink ref="A149" display="README.md" r:id="rId296"/>
+    <hyperlink ref="I149" display="README.md" r:id="rId297"/>
+    <hyperlink ref="A150" display="README.md" r:id="rId298"/>
+    <hyperlink ref="I150" display="README.md" r:id="rId299"/>
+    <hyperlink ref="A151" display="README.md" r:id="rId300"/>
+    <hyperlink ref="I151" display="README.md" r:id="rId301"/>
+    <hyperlink ref="A152" display="README.md" r:id="rId302"/>
+    <hyperlink ref="I152" display="README.md" r:id="rId303"/>
+    <hyperlink ref="A153" display="README.md" r:id="rId304"/>
+    <hyperlink ref="I153" display="README.md" r:id="rId305"/>
+    <hyperlink ref="A154" display="README.md" r:id="rId306"/>
+    <hyperlink ref="I154" display="README.md" r:id="rId307"/>
+    <hyperlink ref="A155" display="README.md" r:id="rId308"/>
+    <hyperlink ref="I155" display="README.md" r:id="rId309"/>
+    <hyperlink ref="A156" display="template.md" r:id="rId310"/>
+    <hyperlink ref="I156" display="template.md" r:id="rId311"/>
+    <hyperlink ref="A157" display="voice-tone.md" r:id="rId312"/>
+    <hyperlink ref="I157" display="voice-tone.md" r:id="rId313"/>
+    <hyperlink ref="A158" display="TOC.md" r:id="rId314"/>
+    <hyperlink ref="I158" display="TOC.md" r:id="rId315"/>
+    <hyperlink ref="A159" display="CONTRIBUTING.md" r:id="rId316"/>
+    <hyperlink ref="A160" display="applications.md" r:id="rId317"/>
+    <hyperlink ref="A161" display="nuget-packages.md" r:id="rId318"/>
+    <hyperlink ref="A162" display="cli-console-app-tutorial-advanced.md" r:id="rId319"/>
+    <hyperlink ref="A163" display="libraries-with-vs.md" r:id="rId320"/>
+    <hyperlink ref="A164" display="servicing.md" r:id="rId321"/>
+    <hyperlink ref="A165" display="codedoc.md" r:id="rId322"/>
+    <hyperlink ref="A166" display="concepts.md" r:id="rId323"/>
+    <hyperlink ref="A167" display="features.md" r:id="rId324"/>
+    <hyperlink ref="A168" display="generics.md" r:id="rId325"/>
+    <hyperlink ref="A169" display="index.md" r:id="rId326"/>
+    <hyperlink ref="A170" display="interop.md" r:id="rId327"/>
+    <hyperlink ref="A171" display="lambda-expressions.md" r:id="rId328"/>
+    <hyperlink ref="A172" display="linq.md" r:id="rId329"/>
+    <hyperlink ref="A173" display="parallel.md" r:id="rId330"/>
+    <hyperlink ref="A174" display="reflection.md" r:id="rId331"/>
+    <hyperlink ref="A175" display="syntax.md" r:id="rId332"/>
+    <hyperlink ref="A176" display="type-system.md" r:id="rId333"/>
+    <hyperlink ref="A177" display="toc.md" r:id="rId334"/>
   </hyperlinks>
   <headerFooter/>
   <tableParts>

</xml_diff>